<commit_message>
Figure 6 table completed
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Figure_22" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure_6" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure_22" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,6 +394,11 @@
           <t>White</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -400,35 +406,26 @@
           <t>Imperial</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>32%</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>54%</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>66%</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
+      <c r="B2">
+        <v>5.1</v>
+      </c>
+      <c r="C2">
+        <v>15.7</v>
+      </c>
+      <c r="D2">
+        <v>6.8</v>
+      </c>
+      <c r="E2">
+        <v>3.1</v>
+      </c>
+      <c r="F2">
+        <v>11.3</v>
+      </c>
+      <c r="G2">
+        <v>4.5</v>
+      </c>
+      <c r="H2">
+        <v>6.6</v>
       </c>
     </row>
     <row r="3">
@@ -437,35 +434,26 @@
           <t>Los Angeles</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>54%</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>39%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>40%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>40%</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>54%</t>
-        </is>
+      <c r="B3">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="C3">
+        <v>16.2</v>
+      </c>
+      <c r="D3">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E3">
+        <v>8.9</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>7.3</v>
+      </c>
+      <c r="H3">
+        <v>8.6</v>
       </c>
     </row>
     <row r="4">
@@ -474,35 +462,26 @@
           <t>Orange</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>39%</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>54%</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="B4">
+        <v>5.6</v>
+      </c>
+      <c r="C4">
+        <v>9.4</v>
+      </c>
+      <c r="D4">
+        <v>4.2</v>
+      </c>
+      <c r="E4">
+        <v>3.8</v>
+      </c>
+      <c r="F4">
+        <v>4.8</v>
+      </c>
+      <c r="G4">
+        <v>4.2</v>
+      </c>
+      <c r="H4">
+        <v>4.6</v>
       </c>
     </row>
     <row r="5">
@@ -511,35 +490,26 @@
           <t>Riverside</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>52%</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="B5">
+        <v>3.9</v>
+      </c>
+      <c r="C5">
+        <v>5.9</v>
+      </c>
+      <c r="D5">
+        <v>3.4</v>
+      </c>
+      <c r="E5">
+        <v>6.3</v>
+      </c>
+      <c r="F5">
+        <v>10.5</v>
+      </c>
+      <c r="G5">
+        <v>3.9</v>
+      </c>
+      <c r="H5">
+        <v>3.9</v>
       </c>
     </row>
     <row r="6">
@@ -548,35 +518,26 @@
           <t>San Bernardino</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>69%</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>57%</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>52%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>52%</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>69%</t>
-        </is>
+      <c r="B6">
+        <v>4.5</v>
+      </c>
+      <c r="C6">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="D6">
+        <v>3.5</v>
+      </c>
+      <c r="E6">
+        <v>6.1</v>
+      </c>
+      <c r="F6">
+        <v>6.4</v>
+      </c>
+      <c r="G6">
+        <v>4.8</v>
+      </c>
+      <c r="H6">
+        <v>4.6</v>
       </c>
     </row>
     <row r="7">
@@ -585,35 +546,26 @@
           <t>Ventura</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>77%</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>46%</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>55%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>49%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
+      <c r="B7">
+        <v>3.3</v>
+      </c>
+      <c r="C7">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="D7">
+        <v>4.2</v>
+      </c>
+      <c r="E7">
+        <v>3.2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4.1</v>
+      </c>
+      <c r="H7">
+        <v>4.1</v>
       </c>
     </row>
     <row r="8">
@@ -622,35 +574,277 @@
           <t>SCAG</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>36%</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>45%</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>46%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>49%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>13.7</v>
+      </c>
+      <c r="D8">
+        <v>6.3</v>
+      </c>
+      <c r="E8">
+        <v>7.1</v>
+      </c>
+      <c r="F8">
+        <v>11.1</v>
+      </c>
+      <c r="G8">
+        <v>5.7</v>
+      </c>
+      <c r="H8">
+        <v>6.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>59</v>
+      </c>
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>54</v>
+      </c>
+      <c r="E2">
+        <v>76</v>
+      </c>
+      <c r="F2">
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <v>76</v>
+      </c>
+      <c r="H2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>39</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>65</v>
+      </c>
+      <c r="H4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <v>62</v>
+      </c>
+      <c r="E5">
+        <v>61</v>
+      </c>
+      <c r="F5">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>75</v>
+      </c>
+      <c r="H5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>52</v>
+      </c>
+      <c r="F6">
+        <v>52</v>
+      </c>
+      <c r="G6">
+        <v>69</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>77</v>
+      </c>
+      <c r="C7">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>55</v>
+      </c>
+      <c r="F7">
+        <v>49</v>
+      </c>
+      <c r="G7">
+        <v>71</v>
+      </c>
+      <c r="H7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>46</v>
+      </c>
+      <c r="F8">
+        <v>49</v>
+      </c>
+      <c r="G8">
+        <v>62</v>
+      </c>
+      <c r="H8">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update EOD Tues. Feb. 6th- finished replicating 3 figures total
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Figure_6" sheetId="1" r:id="rId1"/>
-    <sheet name="Figure_22" sheetId="2" r:id="rId2"/>
+    <sheet name="Figure_5" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure_6" sheetId="2" r:id="rId2"/>
+    <sheet name="Figure_22" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -407,25 +408,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>5.1</v>
+        <v>2.18</v>
       </c>
       <c r="C2">
-        <v>15.7</v>
+        <v>14.27</v>
       </c>
       <c r="D2">
-        <v>6.8</v>
+        <v>3.67</v>
       </c>
       <c r="E2">
-        <v>3.1</v>
+        <v>5.19</v>
       </c>
       <c r="F2">
-        <v>11.3</v>
+        <v>5.61</v>
       </c>
       <c r="G2">
-        <v>4.5</v>
+        <v>5.65</v>
       </c>
       <c r="H2">
-        <v>6.6</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="3">
@@ -435,25 +436,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>8.199999999999999</v>
+        <v>7.32</v>
       </c>
       <c r="C3">
-        <v>16.2</v>
+        <v>10.53</v>
       </c>
       <c r="D3">
-        <v>8.199999999999999</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="E3">
+        <v>9.789999999999999</v>
+      </c>
+      <c r="F3">
+        <v>9.550000000000001</v>
+      </c>
+      <c r="G3">
+        <v>7.19</v>
+      </c>
+      <c r="H3">
         <v>8.9</v>
-      </c>
-      <c r="F3">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>7.3</v>
-      </c>
-      <c r="H3">
-        <v>8.6</v>
       </c>
     </row>
     <row r="4">
@@ -463,25 +464,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>5.6</v>
+        <v>3.49</v>
       </c>
       <c r="C4">
-        <v>9.4</v>
+        <v>7.02</v>
       </c>
       <c r="D4">
-        <v>4.2</v>
+        <v>5.94</v>
       </c>
       <c r="E4">
-        <v>3.8</v>
+        <v>3.45</v>
       </c>
       <c r="F4">
-        <v>4.8</v>
+        <v>3.94</v>
       </c>
       <c r="G4">
-        <v>4.2</v>
+        <v>3.45</v>
       </c>
       <c r="H4">
-        <v>4.6</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="5">
@@ -491,25 +492,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>3.9</v>
+        <v>3.89</v>
       </c>
       <c r="C5">
-        <v>5.9</v>
+        <v>3.56</v>
       </c>
       <c r="D5">
-        <v>3.4</v>
+        <v>2.16</v>
       </c>
       <c r="E5">
-        <v>6.3</v>
+        <v>2.99</v>
       </c>
       <c r="F5">
-        <v>10.5</v>
+        <v>9.91</v>
       </c>
       <c r="G5">
-        <v>3.9</v>
+        <v>2.43</v>
       </c>
       <c r="H5">
-        <v>3.9</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="6">
@@ -519,25 +520,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>4.5</v>
+        <v>2.39</v>
       </c>
       <c r="C6">
-        <v>8.699999999999999</v>
+        <v>5.45</v>
       </c>
       <c r="D6">
-        <v>3.5</v>
+        <v>2.78</v>
       </c>
       <c r="E6">
-        <v>6.1</v>
+        <v>4.57</v>
       </c>
       <c r="F6">
-        <v>6.4</v>
+        <v>12.27</v>
       </c>
       <c r="G6">
-        <v>4.8</v>
+        <v>2.99</v>
       </c>
       <c r="H6">
-        <v>4.6</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="7">
@@ -547,25 +548,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>3.3</v>
+        <v>2.67</v>
       </c>
       <c r="C7">
-        <v>8.800000000000001</v>
+        <v>6.14</v>
       </c>
       <c r="D7">
-        <v>4.2</v>
+        <v>3.04</v>
       </c>
       <c r="E7">
-        <v>3.2</v>
+        <v>4.19</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>4.1</v>
+        <v>2.97</v>
       </c>
       <c r="H7">
-        <v>4.1</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="8">
@@ -575,25 +576,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>5.68</v>
       </c>
       <c r="C8">
-        <v>13.7</v>
+        <v>8.73</v>
       </c>
       <c r="D8">
-        <v>6.3</v>
+        <v>7.16</v>
       </c>
       <c r="E8">
-        <v>7.1</v>
+        <v>6.84</v>
       </c>
       <c r="F8">
-        <v>11.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G8">
-        <v>5.7</v>
+        <v>4.99</v>
       </c>
       <c r="H8">
-        <v>6.7</v>
+        <v>6.41</v>
       </c>
     </row>
   </sheetData>
@@ -658,25 +659,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>5.1</v>
       </c>
       <c r="C2">
-        <v>32</v>
+        <v>15.74</v>
       </c>
       <c r="D2">
-        <v>54</v>
+        <v>6.79</v>
       </c>
       <c r="E2">
-        <v>76</v>
+        <v>3.09</v>
       </c>
       <c r="F2">
-        <v>66</v>
+        <v>11.3</v>
       </c>
       <c r="G2">
-        <v>76</v>
+        <v>4.49</v>
       </c>
       <c r="H2">
-        <v>57</v>
+        <v>6.64</v>
       </c>
     </row>
     <row r="3">
@@ -686,25 +687,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>54</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>16.2</v>
       </c>
       <c r="D3">
-        <v>39</v>
+        <v>8.16</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>14.95</v>
       </c>
       <c r="G3">
-        <v>54</v>
+        <v>7.26</v>
       </c>
       <c r="H3">
-        <v>46</v>
+        <v>8.619999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -714,25 +715,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>5.63</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>9.44</v>
       </c>
       <c r="D4">
-        <v>39</v>
+        <v>4.24</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>3.76</v>
       </c>
       <c r="F4">
-        <v>54</v>
+        <v>4.8</v>
       </c>
       <c r="G4">
-        <v>65</v>
+        <v>4.24</v>
       </c>
       <c r="H4">
-        <v>57</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="5">
@@ -742,25 +743,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>3.93</v>
       </c>
       <c r="C5">
-        <v>52</v>
+        <v>5.86</v>
       </c>
       <c r="D5">
-        <v>62</v>
+        <v>3.42</v>
       </c>
       <c r="E5">
-        <v>61</v>
+        <v>6.25</v>
       </c>
       <c r="F5">
-        <v>62</v>
+        <v>10.46</v>
       </c>
       <c r="G5">
-        <v>75</v>
+        <v>3.9</v>
       </c>
       <c r="H5">
-        <v>68</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="6">
@@ -770,25 +771,276 @@
         </is>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>4.46</v>
       </c>
       <c r="C6">
-        <v>38</v>
+        <v>8.66</v>
       </c>
       <c r="D6">
-        <v>57</v>
+        <v>3.54</v>
+      </c>
+      <c r="E6">
+        <v>6.09</v>
+      </c>
+      <c r="F6">
+        <v>6.44</v>
+      </c>
+      <c r="G6">
+        <v>4.78</v>
+      </c>
+      <c r="H6">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>3.26</v>
+      </c>
+      <c r="C7">
+        <v>8.85</v>
+      </c>
+      <c r="D7">
+        <v>4.2</v>
+      </c>
+      <c r="E7">
+        <v>3.2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4.07</v>
+      </c>
+      <c r="H7">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>6.97</v>
+      </c>
+      <c r="C8">
+        <v>13.7</v>
+      </c>
+      <c r="D8">
+        <v>6.31</v>
+      </c>
+      <c r="E8">
+        <v>7.13</v>
+      </c>
+      <c r="F8">
+        <v>11.05</v>
+      </c>
+      <c r="G8">
+        <v>5.68</v>
+      </c>
+      <c r="H8">
+        <v>6.71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>58.67</v>
+      </c>
+      <c r="C2">
+        <v>32.16</v>
+      </c>
+      <c r="D2">
+        <v>54.25</v>
+      </c>
+      <c r="E2">
+        <v>75.68000000000001</v>
+      </c>
+      <c r="F2">
+        <v>65.54000000000001</v>
+      </c>
+      <c r="G2">
+        <v>75.55</v>
+      </c>
+      <c r="H2">
+        <v>57.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>54.25</v>
+      </c>
+      <c r="C3">
+        <v>32.85</v>
+      </c>
+      <c r="D3">
+        <v>39.07</v>
+      </c>
+      <c r="E3">
+        <v>39.94</v>
+      </c>
+      <c r="F3">
+        <v>40.3</v>
+      </c>
+      <c r="G3">
+        <v>53.53</v>
+      </c>
+      <c r="H3">
+        <v>45.81</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>62.37</v>
+      </c>
+      <c r="C4">
+        <v>33.38</v>
+      </c>
+      <c r="D4">
+        <v>38.84</v>
+      </c>
+      <c r="E4">
+        <v>50.27</v>
+      </c>
+      <c r="F4">
+        <v>53.77</v>
+      </c>
+      <c r="G4">
+        <v>64.56999999999999</v>
+      </c>
+      <c r="H4">
+        <v>56.76</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>75.95</v>
+      </c>
+      <c r="C5">
+        <v>52.18</v>
+      </c>
+      <c r="D5">
+        <v>61.73</v>
+      </c>
+      <c r="E5">
+        <v>60.78</v>
+      </c>
+      <c r="F5">
+        <v>61.57</v>
+      </c>
+      <c r="G5">
+        <v>74.83</v>
+      </c>
+      <c r="H5">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>69.15000000000001</v>
+      </c>
+      <c r="C6">
+        <v>37.75</v>
+      </c>
+      <c r="D6">
+        <v>56.87</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6">
-        <v>52</v>
+        <v>52.45</v>
       </c>
       <c r="G6">
-        <v>69</v>
+        <v>68.87</v>
       </c>
       <c r="H6">
-        <v>60</v>
+        <v>60.26</v>
       </c>
     </row>
     <row r="7">
@@ -798,25 +1050,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>77</v>
+        <v>76.79000000000001</v>
       </c>
       <c r="C7">
-        <v>46</v>
+        <v>46.48</v>
       </c>
       <c r="D7">
-        <v>48</v>
+        <v>48.23</v>
       </c>
       <c r="E7">
-        <v>55</v>
+        <v>55.1</v>
       </c>
       <c r="F7">
-        <v>49</v>
+        <v>49.11</v>
       </c>
       <c r="G7">
-        <v>71</v>
+        <v>70.66</v>
       </c>
       <c r="H7">
-        <v>63</v>
+        <v>63.16</v>
       </c>
     </row>
     <row r="8">
@@ -826,25 +1078,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>59</v>
+        <v>58.98</v>
       </c>
       <c r="C8">
-        <v>36</v>
+        <v>35.79</v>
       </c>
       <c r="D8">
-        <v>45</v>
+        <v>44.93</v>
       </c>
       <c r="E8">
-        <v>46</v>
+        <v>46.11</v>
       </c>
       <c r="F8">
-        <v>49</v>
+        <v>48.63</v>
       </c>
       <c r="G8">
-        <v>62</v>
+        <v>61.52</v>
       </c>
       <c r="H8">
-        <v>53</v>
+        <v>52.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Fig 19 and created a TOC for the tabbed excel workbook
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -7,10 +7,12 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Figure_5" sheetId="1" r:id="rId1"/>
-    <sheet name="Figure_6" sheetId="2" r:id="rId2"/>
-    <sheet name="Figure 7" sheetId="3" r:id="rId3"/>
-    <sheet name="Figure_22" sheetId="4" r:id="rId4"/>
+    <sheet name="TOC" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure_5" sheetId="2" r:id="rId2"/>
+    <sheet name="Figure_6" sheetId="3" r:id="rId3"/>
+    <sheet name="Figure_7" sheetId="4" r:id="rId4"/>
+    <sheet name="Figure_19" sheetId="5" r:id="rId5"/>
+    <sheet name="Figure_22" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -354,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -363,239 +365,145 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>county</t>
+          <t>sheet_name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Black</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Hispanic/Latino</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Multiracial/Other</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Native American</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>White</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
+          <t>figure_name</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Imperial</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>2.18</v>
-      </c>
-      <c r="C2">
-        <v>14.27</v>
-      </c>
-      <c r="D2">
-        <v>3.67</v>
-      </c>
-      <c r="E2">
-        <v>5.19</v>
-      </c>
-      <c r="F2">
-        <v>5.61</v>
-      </c>
-      <c r="G2">
-        <v>5.65</v>
-      </c>
-      <c r="H2">
-        <v>4.13</v>
+          <t>Figure_5</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Figure 5. Workers who Commute by Walk, Bike, or Public Transit by Race and Ethnicity</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>7.32</v>
-      </c>
-      <c r="C3">
-        <v>10.53</v>
-      </c>
-      <c r="D3">
-        <v>9.960000000000001</v>
-      </c>
-      <c r="E3">
-        <v>9.789999999999999</v>
-      </c>
-      <c r="F3">
-        <v>9.550000000000001</v>
-      </c>
-      <c r="G3">
-        <v>7.19</v>
-      </c>
-      <c r="H3">
-        <v>8.9</v>
+          <t>Figure_6</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Figure 6. Householders without a Vehicle by Race and Ethnicity</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>3.49</v>
-      </c>
-      <c r="C4">
-        <v>7.02</v>
-      </c>
-      <c r="D4">
-        <v>5.94</v>
-      </c>
-      <c r="E4">
-        <v>3.45</v>
-      </c>
-      <c r="F4">
-        <v>3.94</v>
-      </c>
-      <c r="G4">
-        <v>3.45</v>
-      </c>
-      <c r="H4">
-        <v>4.41</v>
+          <t>Figure_7</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Figure 7. Workers’ Commute Times (Minutes) by Mode and Race and Ethnicity</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Riverside</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>3.89</v>
-      </c>
-      <c r="C5">
-        <v>3.56</v>
-      </c>
-      <c r="D5">
-        <v>2.16</v>
-      </c>
-      <c r="E5">
-        <v>2.99</v>
-      </c>
-      <c r="F5">
-        <v>9.91</v>
-      </c>
-      <c r="G5">
-        <v>2.43</v>
-      </c>
-      <c r="H5">
-        <v>2.49</v>
+          <t>Figure_19</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Figure 19. Renters and Homeowners Experiencing Housing Cost Burden by Race and Ethnicity</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>San Bernardino</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>2.39</v>
-      </c>
-      <c r="C6">
-        <v>5.45</v>
-      </c>
-      <c r="D6">
-        <v>2.78</v>
-      </c>
-      <c r="E6">
-        <v>4.57</v>
-      </c>
-      <c r="F6">
-        <v>12.27</v>
-      </c>
-      <c r="G6">
-        <v>2.99</v>
-      </c>
-      <c r="H6">
-        <v>3.07</v>
+          <t>Figure_20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Figure 20. People Living in Households Without Kitchen and Plumbing Facilities by Race and Ethnicity</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ventura</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>2.67</v>
-      </c>
-      <c r="C7">
-        <v>6.14</v>
-      </c>
-      <c r="D7">
-        <v>3.04</v>
-      </c>
-      <c r="E7">
-        <v>4.19</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>2.97</v>
-      </c>
-      <c r="H7">
-        <v>3.07</v>
+          <t>Figure_21</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Figure 21. Households with Severe Overcrowding by Race and Ethniciy</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SCAG</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>5.68</v>
-      </c>
-      <c r="C8">
-        <v>8.73</v>
-      </c>
-      <c r="D8">
-        <v>7.16</v>
-      </c>
-      <c r="E8">
-        <v>6.84</v>
-      </c>
-      <c r="F8">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="G8">
-        <v>4.99</v>
-      </c>
-      <c r="H8">
-        <v>6.41</v>
+          <t>Figure_22</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Figure 22. Homeownership by Race and Ethniciy</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Figure_28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Figure 28. People without Health Insurance by Race and Ethnicity</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Figure_39</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Figure 39. Median Hourly Wage by Race and Ethnicity</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Figure_40</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Figure 40. Unemployment by Race and Ethnicity</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Figure_41</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Figure 41. Working Poor by Race and Ethnicity</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -660,25 +568,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>5.1</v>
+        <v>2.18</v>
       </c>
       <c r="C2">
-        <v>15.74</v>
+        <v>14.27</v>
       </c>
       <c r="D2">
-        <v>6.79</v>
+        <v>3.67</v>
       </c>
       <c r="E2">
-        <v>3.09</v>
+        <v>5.19</v>
       </c>
       <c r="F2">
-        <v>11.3</v>
+        <v>5.61</v>
       </c>
       <c r="G2">
-        <v>4.49</v>
+        <v>5.65</v>
       </c>
       <c r="H2">
-        <v>6.64</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="3">
@@ -688,25 +596,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>8.220000000000001</v>
+        <v>7.32</v>
       </c>
       <c r="C3">
-        <v>16.2</v>
+        <v>10.53</v>
       </c>
       <c r="D3">
-        <v>8.16</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="E3">
-        <v>8.869999999999999</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="F3">
-        <v>14.95</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="G3">
-        <v>7.26</v>
+        <v>7.19</v>
       </c>
       <c r="H3">
-        <v>8.619999999999999</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="4">
@@ -716,25 +624,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>5.63</v>
+        <v>3.49</v>
       </c>
       <c r="C4">
-        <v>9.44</v>
+        <v>7.02</v>
       </c>
       <c r="D4">
-        <v>4.24</v>
+        <v>5.94</v>
       </c>
       <c r="E4">
-        <v>3.76</v>
+        <v>3.45</v>
       </c>
       <c r="F4">
-        <v>4.8</v>
+        <v>3.94</v>
       </c>
       <c r="G4">
-        <v>4.24</v>
+        <v>3.45</v>
       </c>
       <c r="H4">
-        <v>4.6</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="5">
@@ -744,25 +652,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>3.93</v>
+        <v>3.89</v>
       </c>
       <c r="C5">
-        <v>5.86</v>
+        <v>3.56</v>
       </c>
       <c r="D5">
-        <v>3.42</v>
+        <v>2.16</v>
       </c>
       <c r="E5">
-        <v>6.25</v>
+        <v>2.99</v>
       </c>
       <c r="F5">
-        <v>10.46</v>
+        <v>9.91</v>
       </c>
       <c r="G5">
-        <v>3.9</v>
+        <v>2.43</v>
       </c>
       <c r="H5">
-        <v>3.93</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="6">
@@ -772,25 +680,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>4.46</v>
+        <v>2.39</v>
       </c>
       <c r="C6">
-        <v>8.66</v>
+        <v>5.45</v>
       </c>
       <c r="D6">
-        <v>3.54</v>
+        <v>2.78</v>
       </c>
       <c r="E6">
-        <v>6.09</v>
+        <v>4.57</v>
       </c>
       <c r="F6">
-        <v>6.44</v>
+        <v>12.27</v>
       </c>
       <c r="G6">
-        <v>4.78</v>
+        <v>2.99</v>
       </c>
       <c r="H6">
-        <v>4.57</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="7">
@@ -800,25 +708,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>3.26</v>
+        <v>2.67</v>
       </c>
       <c r="C7">
-        <v>8.85</v>
+        <v>6.14</v>
       </c>
       <c r="D7">
-        <v>4.2</v>
+        <v>3.04</v>
       </c>
       <c r="E7">
-        <v>3.2</v>
+        <v>4.19</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>4.07</v>
+        <v>2.97</v>
       </c>
       <c r="H7">
-        <v>4.1</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="8">
@@ -828,25 +736,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>6.97</v>
+        <v>5.68</v>
       </c>
       <c r="C8">
-        <v>13.7</v>
+        <v>8.73</v>
       </c>
       <c r="D8">
-        <v>6.31</v>
+        <v>7.16</v>
       </c>
       <c r="E8">
-        <v>7.13</v>
+        <v>6.84</v>
       </c>
       <c r="F8">
-        <v>11.05</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G8">
-        <v>5.68</v>
+        <v>4.99</v>
       </c>
       <c r="H8">
-        <v>6.71</v>
+        <v>6.41</v>
       </c>
     </row>
   </sheetData>
@@ -855,6 +763,257 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>5.1</v>
+      </c>
+      <c r="C2">
+        <v>15.74</v>
+      </c>
+      <c r="D2">
+        <v>6.79</v>
+      </c>
+      <c r="E2">
+        <v>3.09</v>
+      </c>
+      <c r="F2">
+        <v>11.3</v>
+      </c>
+      <c r="G2">
+        <v>4.49</v>
+      </c>
+      <c r="H2">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="C3">
+        <v>16.2</v>
+      </c>
+      <c r="D3">
+        <v>8.16</v>
+      </c>
+      <c r="E3">
+        <v>8.869999999999999</v>
+      </c>
+      <c r="F3">
+        <v>14.95</v>
+      </c>
+      <c r="G3">
+        <v>7.26</v>
+      </c>
+      <c r="H3">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>5.63</v>
+      </c>
+      <c r="C4">
+        <v>9.44</v>
+      </c>
+      <c r="D4">
+        <v>4.24</v>
+      </c>
+      <c r="E4">
+        <v>3.76</v>
+      </c>
+      <c r="F4">
+        <v>4.8</v>
+      </c>
+      <c r="G4">
+        <v>4.24</v>
+      </c>
+      <c r="H4">
+        <v>4.6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>3.93</v>
+      </c>
+      <c r="C5">
+        <v>5.86</v>
+      </c>
+      <c r="D5">
+        <v>3.42</v>
+      </c>
+      <c r="E5">
+        <v>6.25</v>
+      </c>
+      <c r="F5">
+        <v>10.46</v>
+      </c>
+      <c r="G5">
+        <v>3.9</v>
+      </c>
+      <c r="H5">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>4.46</v>
+      </c>
+      <c r="C6">
+        <v>8.66</v>
+      </c>
+      <c r="D6">
+        <v>3.54</v>
+      </c>
+      <c r="E6">
+        <v>6.09</v>
+      </c>
+      <c r="F6">
+        <v>6.44</v>
+      </c>
+      <c r="G6">
+        <v>4.78</v>
+      </c>
+      <c r="H6">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>3.26</v>
+      </c>
+      <c r="C7">
+        <v>8.85</v>
+      </c>
+      <c r="D7">
+        <v>4.2</v>
+      </c>
+      <c r="E7">
+        <v>3.2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4.07</v>
+      </c>
+      <c r="H7">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>6.97</v>
+      </c>
+      <c r="C8">
+        <v>13.7</v>
+      </c>
+      <c r="D8">
+        <v>6.31</v>
+      </c>
+      <c r="E8">
+        <v>7.13</v>
+      </c>
+      <c r="F8">
+        <v>11.05</v>
+      </c>
+      <c r="G8">
+        <v>5.68</v>
+      </c>
+      <c r="H8">
+        <v>6.71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F44"/>
   <sheetViews>
@@ -906,16 +1065,16 @@
         </is>
       </c>
       <c r="C2">
-        <v>20.44867764009617</v>
+        <v>20.45</v>
       </c>
       <c r="D2">
-        <v>52.82244850862516</v>
+        <v>52.82</v>
       </c>
       <c r="E2">
-        <v>30.81357572893418</v>
+        <v>30.81</v>
       </c>
       <c r="F2">
-        <v>31.10350496615202</v>
+        <v>31.1</v>
       </c>
     </row>
     <row r="3">
@@ -930,16 +1089,16 @@
         </is>
       </c>
       <c r="C3">
-        <v>22.08103578765272</v>
+        <v>22.08</v>
       </c>
       <c r="D3">
-        <v>56.00406848066658</v>
+        <v>56</v>
       </c>
       <c r="E3">
-        <v>32.60097169625794</v>
+        <v>32.6</v>
       </c>
       <c r="F3">
-        <v>33.77724471120202</v>
+        <v>33.78</v>
       </c>
     </row>
     <row r="4">
@@ -954,16 +1113,16 @@
         </is>
       </c>
       <c r="C4">
-        <v>19.49316522893165</v>
+        <v>19.49</v>
       </c>
       <c r="D4">
-        <v>49.43096984247048</v>
+        <v>49.43</v>
       </c>
       <c r="E4">
-        <v>30.24067811867948</v>
+        <v>30.24</v>
       </c>
       <c r="F4">
-        <v>30.7613245280496</v>
+        <v>30.76</v>
       </c>
     </row>
     <row r="5">
@@ -978,16 +1137,16 @@
         </is>
       </c>
       <c r="C5">
-        <v>18.75136726966765</v>
+        <v>18.75</v>
       </c>
       <c r="D5">
-        <v>48.37766703005762</v>
+        <v>48.38</v>
       </c>
       <c r="E5">
-        <v>30.73713943066338</v>
+        <v>30.74</v>
       </c>
       <c r="F5">
-        <v>30.59712986153093</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="6">
@@ -1002,16 +1161,16 @@
         </is>
       </c>
       <c r="C6">
-        <v>21.18838992332968</v>
+        <v>21.19</v>
       </c>
       <c r="D6">
-        <v>74.27477477477477</v>
+        <v>74.27</v>
       </c>
       <c r="E6">
-        <v>31.98979819792985</v>
+        <v>31.99</v>
       </c>
       <c r="F6">
-        <v>33.20915511727079</v>
+        <v>33.21</v>
       </c>
     </row>
     <row r="7">
@@ -1026,16 +1185,16 @@
         </is>
       </c>
       <c r="C7">
-        <v>19.07920958131092</v>
+        <v>19.08</v>
       </c>
       <c r="D7">
-        <v>52.71617010557171</v>
+        <v>52.72</v>
       </c>
       <c r="E7">
-        <v>30.08533204448237</v>
+        <v>30.09</v>
       </c>
       <c r="F7">
-        <v>30.02899968827999</v>
+        <v>30.03</v>
       </c>
     </row>
     <row r="8">
@@ -1050,16 +1209,16 @@
         </is>
       </c>
       <c r="C8">
-        <v>19.61844171229249</v>
+        <v>19.62</v>
       </c>
       <c r="D8">
-        <v>51.01429403923828</v>
+        <v>51.01</v>
       </c>
       <c r="E8">
-        <v>30.42236330046065</v>
+        <v>30.42</v>
       </c>
       <c r="F8">
-        <v>30.76931574176582</v>
+        <v>30.77</v>
       </c>
     </row>
     <row r="9">
@@ -1074,16 +1233,16 @@
         </is>
       </c>
       <c r="C9">
-        <v>16.27906976744186</v>
+        <v>16.28</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>31.76086956521739</v>
+        <v>31.76</v>
       </c>
       <c r="F9">
-        <v>31.03489640130861</v>
+        <v>31.03</v>
       </c>
     </row>
     <row r="10">
@@ -1098,16 +1257,16 @@
         </is>
       </c>
       <c r="C10">
-        <v>17.65109713387178</v>
+        <v>17.65</v>
       </c>
       <c r="D10">
-        <v>52.03642917133259</v>
+        <v>52.04</v>
       </c>
       <c r="E10">
-        <v>31.05200062436427</v>
+        <v>31.05</v>
       </c>
       <c r="F10">
-        <v>31.40328918256715</v>
+        <v>31.4</v>
       </c>
     </row>
     <row r="11">
@@ -1122,16 +1281,16 @@
         </is>
       </c>
       <c r="C11">
-        <v>27.70311044887316</v>
+        <v>27.7</v>
       </c>
       <c r="D11">
-        <v>54.63176696894751</v>
+        <v>54.63</v>
       </c>
       <c r="E11">
-        <v>29.10496307822044</v>
+        <v>29.1</v>
       </c>
       <c r="F11">
-        <v>29.38062016601977</v>
+        <v>29.38</v>
       </c>
     </row>
     <row r="12">
@@ -1146,16 +1305,16 @@
         </is>
       </c>
       <c r="C12">
-        <v>19.39827856025039</v>
+        <v>19.4</v>
       </c>
       <c r="D12">
-        <v>53.5253227408143</v>
+        <v>53.53</v>
       </c>
       <c r="E12">
-        <v>35.04524310202001</v>
+        <v>35.05</v>
       </c>
       <c r="F12">
-        <v>34.72287630964046</v>
+        <v>34.72</v>
       </c>
     </row>
     <row r="13">
@@ -1170,16 +1329,16 @@
         </is>
       </c>
       <c r="C13">
-        <v>18.61322463768116</v>
+        <v>18.61</v>
       </c>
       <c r="D13">
-        <v>67.24290780141844</v>
+        <v>67.23999999999999</v>
       </c>
       <c r="E13">
-        <v>32.74977473418634</v>
+        <v>32.75</v>
       </c>
       <c r="F13">
-        <v>33.08836094158675</v>
+        <v>33.09</v>
       </c>
     </row>
     <row r="14">
@@ -1194,16 +1353,16 @@
         </is>
       </c>
       <c r="C14">
-        <v>26.78031212484994</v>
+        <v>26.78</v>
       </c>
       <c r="D14">
-        <v>49.35126582278481</v>
+        <v>49.35</v>
       </c>
       <c r="E14">
-        <v>27.87183629509962</v>
+        <v>27.87</v>
       </c>
       <c r="F14">
-        <v>28.08837072236343</v>
+        <v>28.09</v>
       </c>
     </row>
     <row r="15">
@@ -1218,16 +1377,16 @@
         </is>
       </c>
       <c r="C15">
-        <v>24.10752688172043</v>
+        <v>24.11</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>19.55970924195223</v>
+        <v>19.56</v>
       </c>
       <c r="F15">
-        <v>20.29590948651001</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="16">
@@ -1242,16 +1401,16 @@
         </is>
       </c>
       <c r="C16">
-        <v>22.3332344653715</v>
+        <v>22.33</v>
       </c>
       <c r="D16">
-        <v>55.44614622623538</v>
+        <v>55.45</v>
       </c>
       <c r="E16">
-        <v>31.96130062608736</v>
+        <v>31.96</v>
       </c>
       <c r="F16">
-        <v>33.58880727316515</v>
+        <v>33.59</v>
       </c>
     </row>
     <row r="17">
@@ -1266,16 +1425,16 @@
         </is>
       </c>
       <c r="C17">
-        <v>17.83267973856209</v>
+        <v>17.83</v>
       </c>
       <c r="D17">
-        <v>45.3623693379791</v>
+        <v>45.36</v>
       </c>
       <c r="E17">
-        <v>27.87553047614606</v>
+        <v>27.88</v>
       </c>
       <c r="F17">
-        <v>28.4061054975167</v>
+        <v>28.41</v>
       </c>
     </row>
     <row r="18">
@@ -1290,16 +1449,16 @@
         </is>
       </c>
       <c r="C18">
-        <v>27.4481981981982</v>
+        <v>27.45</v>
       </c>
       <c r="D18">
-        <v>64.07168784029038</v>
+        <v>64.06999999999999</v>
       </c>
       <c r="E18">
-        <v>37.11923637859466</v>
+        <v>37.12</v>
       </c>
       <c r="F18">
-        <v>37.34148332150461</v>
+        <v>37.34</v>
       </c>
     </row>
     <row r="19">
@@ -1314,16 +1473,16 @@
         </is>
       </c>
       <c r="C19">
-        <v>16.15207373271889</v>
+        <v>16.15</v>
       </c>
       <c r="D19">
-        <v>66.44417938931298</v>
+        <v>66.44</v>
       </c>
       <c r="E19">
-        <v>33.72317907153454</v>
+        <v>33.72</v>
       </c>
       <c r="F19">
-        <v>34.30081081536672</v>
+        <v>34.3</v>
       </c>
     </row>
     <row r="20">
@@ -1338,16 +1497,16 @@
         </is>
       </c>
       <c r="C20">
-        <v>26.6566265060241</v>
+        <v>26.66</v>
       </c>
       <c r="D20">
-        <v>26.13740458015267</v>
+        <v>26.14</v>
       </c>
       <c r="E20">
-        <v>28.757016840417</v>
+        <v>28.76</v>
       </c>
       <c r="F20">
-        <v>28.60167214093759</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="21">
@@ -1362,16 +1521,16 @@
         </is>
       </c>
       <c r="C21">
-        <v>13.67281420765027</v>
+        <v>13.67</v>
       </c>
       <c r="D21">
-        <v>29.69221105527638</v>
+        <v>29.69</v>
       </c>
       <c r="E21">
-        <v>22.99387969781008</v>
+        <v>22.99</v>
       </c>
       <c r="F21">
-        <v>22.80529849392125</v>
+        <v>22.81</v>
       </c>
     </row>
     <row r="22">
@@ -1386,16 +1545,16 @@
         </is>
       </c>
       <c r="C22">
-        <v>19.32721094287681</v>
+        <v>19.33</v>
       </c>
       <c r="D22">
-        <v>49.30509176032385</v>
+        <v>49.31</v>
       </c>
       <c r="E22">
-        <v>30.62563494424906</v>
+        <v>30.63</v>
       </c>
       <c r="F22">
-        <v>31.4941147340975</v>
+        <v>31.49</v>
       </c>
     </row>
     <row r="23">
@@ -1410,16 +1569,16 @@
         </is>
       </c>
       <c r="C23">
-        <v>18.75576708270604</v>
+        <v>18.76</v>
       </c>
       <c r="D23">
-        <v>46.75181842672414</v>
+        <v>46.75</v>
       </c>
       <c r="E23">
-        <v>26.22257094198571</v>
+        <v>26.22</v>
       </c>
       <c r="F23">
-        <v>26.53241284823276</v>
+        <v>26.53</v>
       </c>
     </row>
     <row r="24">
@@ -1434,16 +1593,16 @@
         </is>
       </c>
       <c r="C24">
-        <v>24.22055239642567</v>
+        <v>24.22</v>
       </c>
       <c r="D24">
-        <v>47.40831492267524</v>
+        <v>47.41</v>
       </c>
       <c r="E24">
-        <v>32.93531240534446</v>
+        <v>32.94</v>
       </c>
       <c r="F24">
-        <v>32.86383314694427</v>
+        <v>32.86</v>
       </c>
     </row>
     <row r="25">
@@ -1458,16 +1617,16 @@
         </is>
       </c>
       <c r="C25">
-        <v>18.82110207162627</v>
+        <v>18.82</v>
       </c>
       <c r="D25">
-        <v>64.95972908658247</v>
+        <v>64.95999999999999</v>
       </c>
       <c r="E25">
-        <v>32.15675496469184</v>
+        <v>32.16</v>
       </c>
       <c r="F25">
-        <v>32.19975267702642</v>
+        <v>32.2</v>
       </c>
     </row>
     <row r="26">
@@ -1482,16 +1641,16 @@
         </is>
       </c>
       <c r="C26">
-        <v>16.65045045045045</v>
+        <v>16.65</v>
       </c>
       <c r="D26">
-        <v>49.54492415402567</v>
+        <v>49.54</v>
       </c>
       <c r="E26">
-        <v>25.36034759672512</v>
+        <v>25.36</v>
       </c>
       <c r="F26">
-        <v>25.40830787642113</v>
+        <v>25.41</v>
       </c>
     </row>
     <row r="27">
@@ -1512,10 +1671,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>13.45771144278607</v>
+        <v>13.46</v>
       </c>
       <c r="F27">
-        <v>13.0188679245283</v>
+        <v>13.02</v>
       </c>
     </row>
     <row r="28">
@@ -1530,16 +1689,16 @@
         </is>
       </c>
       <c r="C28">
-        <v>18.48370241353571</v>
+        <v>18.48</v>
       </c>
       <c r="D28">
-        <v>45.82606188737267</v>
+        <v>45.83</v>
       </c>
       <c r="E28">
-        <v>30.81568668848306</v>
+        <v>30.82</v>
       </c>
       <c r="F28">
-        <v>30.62095377462467</v>
+        <v>30.62</v>
       </c>
     </row>
     <row r="29">
@@ -1554,16 +1713,16 @@
         </is>
       </c>
       <c r="C29">
-        <v>16.9637573964497</v>
+        <v>16.96</v>
       </c>
       <c r="D29">
-        <v>44.40163934426229</v>
+        <v>44.4</v>
       </c>
       <c r="E29">
-        <v>27.547057796403</v>
+        <v>27.55</v>
       </c>
       <c r="F29">
-        <v>27.40196522693124</v>
+        <v>27.4</v>
       </c>
     </row>
     <row r="30">
@@ -1578,16 +1737,16 @@
         </is>
       </c>
       <c r="C30">
-        <v>23.28724832214765</v>
+        <v>23.29</v>
       </c>
       <c r="D30">
-        <v>61.96969696969697</v>
+        <v>61.97</v>
       </c>
       <c r="E30">
-        <v>36.92912782015579</v>
+        <v>36.93</v>
       </c>
       <c r="F30">
-        <v>36.88765694417616</v>
+        <v>36.89</v>
       </c>
     </row>
     <row r="31">
@@ -1602,16 +1761,16 @@
         </is>
       </c>
       <c r="C31">
-        <v>22.58523592085236</v>
+        <v>22.59</v>
       </c>
       <c r="D31">
-        <v>85.57446808510639</v>
+        <v>85.56999999999999</v>
       </c>
       <c r="E31">
-        <v>31.12326232386013</v>
+        <v>31.12</v>
       </c>
       <c r="F31">
-        <v>31.30569399726547</v>
+        <v>31.31</v>
       </c>
     </row>
     <row r="32">
@@ -1626,16 +1785,16 @@
         </is>
       </c>
       <c r="C32">
-        <v>10.18599033816425</v>
+        <v>10.19</v>
       </c>
       <c r="D32">
-        <v>45.94117647058823</v>
+        <v>45.94</v>
       </c>
       <c r="E32">
-        <v>26.95830107289017</v>
+        <v>26.96</v>
       </c>
       <c r="F32">
-        <v>26.39958071278826</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="33">
@@ -1650,7 +1809,7 @@
         </is>
       </c>
       <c r="C33">
-        <v>10.80952380952381</v>
+        <v>10.81</v>
       </c>
       <c r="D33">
         <v>21.25</v>
@@ -1659,7 +1818,7 @@
         <v>24.24</v>
       </c>
       <c r="F33">
-        <v>22.99339933993399</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="34">
@@ -1674,16 +1833,16 @@
         </is>
       </c>
       <c r="C34">
-        <v>17.122</v>
+        <v>17.12</v>
       </c>
       <c r="D34">
-        <v>77.46534653465346</v>
+        <v>77.47</v>
       </c>
       <c r="E34">
-        <v>34.38103727714748</v>
+        <v>34.38</v>
       </c>
       <c r="F34">
-        <v>35.01563172235767</v>
+        <v>35.02</v>
       </c>
     </row>
     <row r="35">
@@ -1698,16 +1857,16 @@
         </is>
       </c>
       <c r="C35">
-        <v>48.68421052631579</v>
+        <v>48.68</v>
       </c>
       <c r="D35">
-        <v>51.70212765957447</v>
+        <v>51.7</v>
       </c>
       <c r="E35">
-        <v>34.47819148936171</v>
+        <v>34.48</v>
       </c>
       <c r="F35">
-        <v>35.42136794807789</v>
+        <v>35.42</v>
       </c>
     </row>
     <row r="36">
@@ -1722,16 +1881,16 @@
         </is>
       </c>
       <c r="C36">
-        <v>1.868421052631579</v>
+        <v>1.87</v>
       </c>
       <c r="D36">
-        <v>77.44845360824742</v>
+        <v>77.45</v>
       </c>
       <c r="E36">
-        <v>38.93649289099526</v>
+        <v>38.94</v>
       </c>
       <c r="F36">
-        <v>41.52519214346712</v>
+        <v>41.53</v>
       </c>
     </row>
     <row r="37">
@@ -1746,16 +1905,16 @@
         </is>
       </c>
       <c r="C37">
-        <v>25.5875486381323</v>
+        <v>25.59</v>
       </c>
       <c r="D37">
         <v>90</v>
       </c>
       <c r="E37">
-        <v>20.23583093179635</v>
+        <v>20.24</v>
       </c>
       <c r="F37">
-        <v>23.1668731928955</v>
+        <v>23.17</v>
       </c>
     </row>
     <row r="38">
@@ -1776,10 +1935,10 @@
         <v>60</v>
       </c>
       <c r="E38">
-        <v>23.79295624332978</v>
+        <v>23.79</v>
       </c>
       <c r="F38">
-        <v>23.79296066252588</v>
+        <v>23.79</v>
       </c>
     </row>
     <row r="39">
@@ -1794,16 +1953,16 @@
         </is>
       </c>
       <c r="C39">
-        <v>19.82456140350877</v>
+        <v>19.82</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>19.16167166167166</v>
+        <v>19.16</v>
       </c>
       <c r="F39">
-        <v>19.20844939647168</v>
+        <v>19.21</v>
       </c>
     </row>
     <row r="40">
@@ -1818,16 +1977,16 @@
         </is>
       </c>
       <c r="C40">
-        <v>18.55870817798867</v>
+        <v>18.56</v>
       </c>
       <c r="D40">
-        <v>50.45528208552093</v>
+        <v>50.46</v>
       </c>
       <c r="E40">
-        <v>30.43568183662725</v>
+        <v>30.44</v>
       </c>
       <c r="F40">
-        <v>30.36350257960408</v>
+        <v>30.36</v>
       </c>
     </row>
     <row r="41">
@@ -1842,16 +2001,16 @@
         </is>
       </c>
       <c r="C41">
-        <v>20.09823610668367</v>
+        <v>20.1</v>
       </c>
       <c r="D41">
-        <v>56.92783697887456</v>
+        <v>56.93</v>
       </c>
       <c r="E41">
-        <v>27.36500068432422</v>
+        <v>27.37</v>
       </c>
       <c r="F41">
-        <v>27.40542438455627</v>
+        <v>27.41</v>
       </c>
     </row>
     <row r="42">
@@ -1866,16 +2025,16 @@
         </is>
       </c>
       <c r="C42">
-        <v>22.57448178189777</v>
+        <v>22.57</v>
       </c>
       <c r="D42">
-        <v>65.13949716139497</v>
+        <v>65.14</v>
       </c>
       <c r="E42">
-        <v>34.48651969463054</v>
+        <v>34.49</v>
       </c>
       <c r="F42">
-        <v>34.42866613131952</v>
+        <v>34.43</v>
       </c>
     </row>
     <row r="43">
@@ -1890,16 +2049,16 @@
         </is>
       </c>
       <c r="C43">
-        <v>17.88362230260696</v>
+        <v>17.88</v>
       </c>
       <c r="D43">
-        <v>60.91723202170964</v>
+        <v>60.92</v>
       </c>
       <c r="E43">
-        <v>31.57125217488915</v>
+        <v>31.57</v>
       </c>
       <c r="F43">
-        <v>31.2735394881211</v>
+        <v>31.27</v>
       </c>
     </row>
     <row r="44">
@@ -1914,16 +2073,16 @@
         </is>
       </c>
       <c r="C44">
-        <v>17.96638268478011</v>
+        <v>17.97</v>
       </c>
       <c r="D44">
-        <v>59.19551506657323</v>
+        <v>59.2</v>
       </c>
       <c r="E44">
-        <v>26.99978549259614</v>
+        <v>27</v>
       </c>
       <c r="F44">
-        <v>27.04309805161698</v>
+        <v>27.04</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +2090,529 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>household_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>13.58</v>
+      </c>
+      <c r="D2">
+        <v>55.77</v>
+      </c>
+      <c r="E2">
+        <v>49.4</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>15.57</v>
+      </c>
+      <c r="H2">
+        <v>26.18</v>
+      </c>
+      <c r="I2">
+        <v>46.59</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>28.36</v>
+      </c>
+      <c r="D3">
+        <v>37.97</v>
+      </c>
+      <c r="E3">
+        <v>41</v>
+      </c>
+      <c r="F3">
+        <v>27.02</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>23.69</v>
+      </c>
+      <c r="I3">
+        <v>33.47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>30.05</v>
+      </c>
+      <c r="D4">
+        <v>26.04</v>
+      </c>
+      <c r="E4">
+        <v>37.29</v>
+      </c>
+      <c r="F4">
+        <v>20.77</v>
+      </c>
+      <c r="G4">
+        <v>25.19</v>
+      </c>
+      <c r="H4">
+        <v>18.57</v>
+      </c>
+      <c r="I4">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>34.52</v>
+      </c>
+      <c r="D5">
+        <v>36.92</v>
+      </c>
+      <c r="E5">
+        <v>41.73</v>
+      </c>
+      <c r="F5">
+        <v>40.4</v>
+      </c>
+      <c r="G5">
+        <v>38.93</v>
+      </c>
+      <c r="H5">
+        <v>29.66</v>
+      </c>
+      <c r="I5">
+        <v>36.68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>33.73</v>
+      </c>
+      <c r="D6">
+        <v>47.14</v>
+      </c>
+      <c r="E6">
+        <v>41.01</v>
+      </c>
+      <c r="F6">
+        <v>40.77</v>
+      </c>
+      <c r="G6">
+        <v>23.85</v>
+      </c>
+      <c r="H6">
+        <v>31.12</v>
+      </c>
+      <c r="I6">
+        <v>38.59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>19.64</v>
+      </c>
+      <c r="D7">
+        <v>31.59</v>
+      </c>
+      <c r="E7">
+        <v>37.63</v>
+      </c>
+      <c r="F7">
+        <v>18.02</v>
+      </c>
+      <c r="G7">
+        <v>11.18</v>
+      </c>
+      <c r="H7">
+        <v>21.11</v>
+      </c>
+      <c r="I7">
+        <v>28.51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Renters</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>29.08</v>
+      </c>
+      <c r="D8">
+        <v>38.53</v>
+      </c>
+      <c r="E8">
+        <v>40.58</v>
+      </c>
+      <c r="F8">
+        <v>28.04</v>
+      </c>
+      <c r="G8">
+        <v>30.19</v>
+      </c>
+      <c r="H8">
+        <v>23.64</v>
+      </c>
+      <c r="I8">
+        <v>33.16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>9.130000000000001</v>
+      </c>
+      <c r="D9">
+        <v>27.54</v>
+      </c>
+      <c r="E9">
+        <v>20.61</v>
+      </c>
+      <c r="F9">
+        <v>4.08</v>
+      </c>
+      <c r="G9">
+        <v>3.45</v>
+      </c>
+      <c r="H9">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="I9">
+        <v>17.71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>11.03</v>
+      </c>
+      <c r="D10">
+        <v>14.75</v>
+      </c>
+      <c r="E10">
+        <v>15.58</v>
+      </c>
+      <c r="F10">
+        <v>10.44</v>
+      </c>
+      <c r="G10">
+        <v>10.11</v>
+      </c>
+      <c r="H10">
+        <v>9.32</v>
+      </c>
+      <c r="I10">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>9.65</v>
+      </c>
+      <c r="D11">
+        <v>10.35</v>
+      </c>
+      <c r="E11">
+        <v>10.57</v>
+      </c>
+      <c r="F11">
+        <v>8.17</v>
+      </c>
+      <c r="G11">
+        <v>4.03</v>
+      </c>
+      <c r="H11">
+        <v>7.66</v>
+      </c>
+      <c r="I11">
+        <v>8.640000000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>11.15</v>
+      </c>
+      <c r="D12">
+        <v>9.83</v>
+      </c>
+      <c r="E12">
+        <v>18.13</v>
+      </c>
+      <c r="F12">
+        <v>11.68</v>
+      </c>
+      <c r="G12">
+        <v>17.52</v>
+      </c>
+      <c r="H12">
+        <v>11.93</v>
+      </c>
+      <c r="I12">
+        <v>14.04</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>13.18</v>
+      </c>
+      <c r="D13">
+        <v>14.49</v>
+      </c>
+      <c r="E13">
+        <v>15.74</v>
+      </c>
+      <c r="F13">
+        <v>10.25</v>
+      </c>
+      <c r="G13">
+        <v>24.54</v>
+      </c>
+      <c r="H13">
+        <v>11.75</v>
+      </c>
+      <c r="I13">
+        <v>13.73</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>6.94</v>
+      </c>
+      <c r="D14">
+        <v>2.96</v>
+      </c>
+      <c r="E14">
+        <v>11.86</v>
+      </c>
+      <c r="F14">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="G14">
+        <v>20.2</v>
+      </c>
+      <c r="H14">
+        <v>7.88</v>
+      </c>
+      <c r="I14">
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Homeowners</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>10.7</v>
+      </c>
+      <c r="D15">
+        <v>13.62</v>
+      </c>
+      <c r="E15">
+        <v>15.51</v>
+      </c>
+      <c r="F15">
+        <v>10.05</v>
+      </c>
+      <c r="G15">
+        <v>13.68</v>
+      </c>
+      <c r="H15">
+        <v>9.52</v>
+      </c>
+      <c r="I15">
+        <v>11.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Replicated 5 more figures EOD Friday 2/9- email to SCAG.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -12,7 +12,11 @@
     <sheet name="Figure_6" sheetId="3" r:id="rId3"/>
     <sheet name="Figure_7" sheetId="4" r:id="rId4"/>
     <sheet name="Figure_19" sheetId="5" r:id="rId5"/>
-    <sheet name="Figure_22" sheetId="6" r:id="rId6"/>
+    <sheet name="Figure_20" sheetId="6" r:id="rId6"/>
+    <sheet name="Figure_21" sheetId="7" r:id="rId7"/>
+    <sheet name="Figure_22" sheetId="8" r:id="rId8"/>
+    <sheet name="Figure_28" sheetId="9" r:id="rId9"/>
+    <sheet name="Figure_39" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -511,6 +515,257 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>22.67</v>
+      </c>
+      <c r="C2">
+        <v>10.75</v>
+      </c>
+      <c r="D2">
+        <v>15.5</v>
+      </c>
+      <c r="E2">
+        <v>18.55</v>
+      </c>
+      <c r="F2">
+        <v>13.29</v>
+      </c>
+      <c r="G2">
+        <v>22.5</v>
+      </c>
+      <c r="H2">
+        <v>15.85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>25.04</v>
+      </c>
+      <c r="C3">
+        <v>21.49</v>
+      </c>
+      <c r="D3">
+        <v>16.12</v>
+      </c>
+      <c r="E3">
+        <v>25.3</v>
+      </c>
+      <c r="F3">
+        <v>21.47</v>
+      </c>
+      <c r="G3">
+        <v>29.43</v>
+      </c>
+      <c r="H3">
+        <v>20.29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>27.97</v>
+      </c>
+      <c r="C4">
+        <v>24.7</v>
+      </c>
+      <c r="D4">
+        <v>17.52</v>
+      </c>
+      <c r="E4">
+        <v>28.69</v>
+      </c>
+      <c r="F4">
+        <v>24.09</v>
+      </c>
+      <c r="G4">
+        <v>32.24</v>
+      </c>
+      <c r="H4">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>23.77</v>
+      </c>
+      <c r="C5">
+        <v>23.14</v>
+      </c>
+      <c r="D5">
+        <v>17.65</v>
+      </c>
+      <c r="E5">
+        <v>23.14</v>
+      </c>
+      <c r="F5">
+        <v>17.48</v>
+      </c>
+      <c r="G5">
+        <v>26.27</v>
+      </c>
+      <c r="H5">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>24.28</v>
+      </c>
+      <c r="C6">
+        <v>20.59</v>
+      </c>
+      <c r="D6">
+        <v>17.71</v>
+      </c>
+      <c r="E6">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>18.76</v>
+      </c>
+      <c r="G6">
+        <v>24.71</v>
+      </c>
+      <c r="H6">
+        <v>20.07</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>31.36</v>
+      </c>
+      <c r="C7">
+        <v>25.23</v>
+      </c>
+      <c r="D7">
+        <v>16.8</v>
+      </c>
+      <c r="E7">
+        <v>27.79</v>
+      </c>
+      <c r="F7">
+        <v>27.33</v>
+      </c>
+      <c r="G7">
+        <v>29.71</v>
+      </c>
+      <c r="H7">
+        <v>22.56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>25.72</v>
+      </c>
+      <c r="C8">
+        <v>21.51</v>
+      </c>
+      <c r="D8">
+        <v>16.76</v>
+      </c>
+      <c r="E8">
+        <v>25.3</v>
+      </c>
+      <c r="F8">
+        <v>20.91</v>
+      </c>
+      <c r="G8">
+        <v>29.16</v>
+      </c>
+      <c r="H8">
+        <v>21.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>
@@ -2669,6 +2924,508 @@
         </is>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.06</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.91</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.19</v>
+      </c>
+      <c r="C3">
+        <v>0.32</v>
+      </c>
+      <c r="D3">
+        <v>0.25</v>
+      </c>
+      <c r="E3">
+        <v>0.34</v>
+      </c>
+      <c r="F3">
+        <v>0.11</v>
+      </c>
+      <c r="G3">
+        <v>0.19</v>
+      </c>
+      <c r="H3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>0.08</v>
+      </c>
+      <c r="C4">
+        <v>0.02</v>
+      </c>
+      <c r="D4">
+        <v>0.12</v>
+      </c>
+      <c r="E4">
+        <v>0.26</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.04</v>
+      </c>
+      <c r="C5">
+        <v>0.14</v>
+      </c>
+      <c r="D5">
+        <v>0.16</v>
+      </c>
+      <c r="E5">
+        <v>0.26</v>
+      </c>
+      <c r="F5">
+        <v>1.63</v>
+      </c>
+      <c r="G5">
+        <v>0.19</v>
+      </c>
+      <c r="H5">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.39</v>
+      </c>
+      <c r="C6">
+        <v>0.29</v>
+      </c>
+      <c r="D6">
+        <v>0.14</v>
+      </c>
+      <c r="E6">
+        <v>0.12</v>
+      </c>
+      <c r="F6">
+        <v>0.21</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>0.18</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.11</v>
+      </c>
+      <c r="E7">
+        <v>0.09</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.15</v>
+      </c>
+      <c r="H7">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>0.17</v>
+      </c>
+      <c r="C8">
+        <v>0.28</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>0.27</v>
+      </c>
+      <c r="F8">
+        <v>0.41</v>
+      </c>
+      <c r="G8">
+        <v>0.16</v>
+      </c>
+      <c r="H8">
+        <v>0.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1.15</v>
+      </c>
+      <c r="C2">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="D2">
+        <v>5.34</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>3.11</v>
+      </c>
+      <c r="G2">
+        <v>0.57</v>
+      </c>
+      <c r="H2">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>5.37</v>
+      </c>
+      <c r="C3">
+        <v>2.69</v>
+      </c>
+      <c r="D3">
+        <v>11.13</v>
+      </c>
+      <c r="E3">
+        <v>2.95</v>
+      </c>
+      <c r="F3">
+        <v>1.56</v>
+      </c>
+      <c r="G3">
+        <v>1.58</v>
+      </c>
+      <c r="H3">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>3.65</v>
+      </c>
+      <c r="C4">
+        <v>2.46</v>
+      </c>
+      <c r="D4">
+        <v>11.31</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2.17</v>
+      </c>
+      <c r="G4">
+        <v>1.2</v>
+      </c>
+      <c r="H4">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2.79</v>
+      </c>
+      <c r="C5">
+        <v>2.18</v>
+      </c>
+      <c r="D5">
+        <v>5.58</v>
+      </c>
+      <c r="E5">
+        <v>2.74</v>
+      </c>
+      <c r="F5">
+        <v>1.14</v>
+      </c>
+      <c r="G5">
+        <v>0.77</v>
+      </c>
+      <c r="H5">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>3.06</v>
+      </c>
+      <c r="C6">
+        <v>2.26</v>
+      </c>
+      <c r="D6">
+        <v>5.77</v>
+      </c>
+      <c r="E6">
+        <v>2.42</v>
+      </c>
+      <c r="F6">
+        <v>2.54</v>
+      </c>
+      <c r="G6">
+        <v>1.13</v>
+      </c>
+      <c r="H6">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>2.98</v>
+      </c>
+      <c r="C7">
+        <v>2.17</v>
+      </c>
+      <c r="D7">
+        <v>7.51</v>
+      </c>
+      <c r="E7">
+        <v>1.05</v>
+      </c>
+      <c r="F7">
+        <v>0.49</v>
+      </c>
+      <c r="G7">
+        <v>0.55</v>
+      </c>
+      <c r="H7">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>4.59</v>
+      </c>
+      <c r="C8">
+        <v>2.58</v>
+      </c>
+      <c r="D8">
+        <v>9.5</v>
+      </c>
+      <c r="E8">
+        <v>2.62</v>
+      </c>
+      <c r="F8">
+        <v>1.68</v>
+      </c>
+      <c r="G8">
+        <v>1.27</v>
+      </c>
+      <c r="H8">
+        <v>4.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
         <v>58.67</v>
       </c>
       <c r="C2">
@@ -2856,6 +3613,257 @@
       </c>
       <c r="H8">
         <v>52.77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="C2">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="D2">
+        <v>6.97</v>
+      </c>
+      <c r="E2">
+        <v>9.449999999999999</v>
+      </c>
+      <c r="F2">
+        <v>13.68</v>
+      </c>
+      <c r="G2">
+        <v>5.53</v>
+      </c>
+      <c r="H2">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>5.55</v>
+      </c>
+      <c r="C3">
+        <v>6.41</v>
+      </c>
+      <c r="D3">
+        <v>13.5</v>
+      </c>
+      <c r="E3">
+        <v>5.43</v>
+      </c>
+      <c r="F3">
+        <v>7.93</v>
+      </c>
+      <c r="G3">
+        <v>4.6</v>
+      </c>
+      <c r="H3">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>4.78</v>
+      </c>
+      <c r="C4">
+        <v>5.95</v>
+      </c>
+      <c r="D4">
+        <v>13.36</v>
+      </c>
+      <c r="E4">
+        <v>4.51</v>
+      </c>
+      <c r="F4">
+        <v>7.36</v>
+      </c>
+      <c r="G4">
+        <v>3.36</v>
+      </c>
+      <c r="H4">
+        <v>7.16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>5.5</v>
+      </c>
+      <c r="C5">
+        <v>6.56</v>
+      </c>
+      <c r="D5">
+        <v>11.71</v>
+      </c>
+      <c r="E5">
+        <v>4.92</v>
+      </c>
+      <c r="F5">
+        <v>19.68</v>
+      </c>
+      <c r="G5">
+        <v>4.73</v>
+      </c>
+      <c r="H5">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>6.08</v>
+      </c>
+      <c r="C6">
+        <v>9.550000000000001</v>
+      </c>
+      <c r="D6">
+        <v>11.9</v>
+      </c>
+      <c r="E6">
+        <v>7.61</v>
+      </c>
+      <c r="F6">
+        <v>11.77</v>
+      </c>
+      <c r="G6">
+        <v>5.74</v>
+      </c>
+      <c r="H6">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>3.71</v>
+      </c>
+      <c r="C7">
+        <v>5.05</v>
+      </c>
+      <c r="D7">
+        <v>15.2</v>
+      </c>
+      <c r="E7">
+        <v>3.46</v>
+      </c>
+      <c r="F7">
+        <v>7.29</v>
+      </c>
+      <c r="G7">
+        <v>3.44</v>
+      </c>
+      <c r="H7">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>5.33</v>
+      </c>
+      <c r="C8">
+        <v>6.85</v>
+      </c>
+      <c r="D8">
+        <v>12.98</v>
+      </c>
+      <c r="E8">
+        <v>5.36</v>
+      </c>
+      <c r="F8">
+        <v>10.92</v>
+      </c>
+      <c r="G8">
+        <v>4.39</v>
+      </c>
+      <c r="H8">
+        <v>8.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed all EA figures- 10 to go from REBCR
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -17,6 +17,8 @@
     <sheet name="Figure_22" sheetId="8" r:id="rId8"/>
     <sheet name="Figure_28" sheetId="9" r:id="rId9"/>
     <sheet name="Figure_39" sheetId="10" r:id="rId10"/>
+    <sheet name="Figure_40" sheetId="11" r:id="rId11"/>
+    <sheet name="Figure_41" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -766,6 +768,508 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>3.54</v>
+      </c>
+      <c r="C2">
+        <v>14.23</v>
+      </c>
+      <c r="D2">
+        <v>16.08</v>
+      </c>
+      <c r="E2">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="F2">
+        <v>8.73</v>
+      </c>
+      <c r="G2">
+        <v>5.06</v>
+      </c>
+      <c r="H2">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>5.48</v>
+      </c>
+      <c r="C3">
+        <v>10.1</v>
+      </c>
+      <c r="D3">
+        <v>6.8</v>
+      </c>
+      <c r="E3">
+        <v>9.1</v>
+      </c>
+      <c r="F3">
+        <v>6.77</v>
+      </c>
+      <c r="G3">
+        <v>6.77</v>
+      </c>
+      <c r="H3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>5.39</v>
+      </c>
+      <c r="C4">
+        <v>8.59</v>
+      </c>
+      <c r="D4">
+        <v>5.44</v>
+      </c>
+      <c r="E4">
+        <v>8.289999999999999</v>
+      </c>
+      <c r="F4">
+        <v>5.73</v>
+      </c>
+      <c r="G4">
+        <v>5.13</v>
+      </c>
+      <c r="H4">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>5.36</v>
+      </c>
+      <c r="C5">
+        <v>10.63</v>
+      </c>
+      <c r="D5">
+        <v>7.74</v>
+      </c>
+      <c r="E5">
+        <v>8.02</v>
+      </c>
+      <c r="F5">
+        <v>10.14</v>
+      </c>
+      <c r="G5">
+        <v>6.44</v>
+      </c>
+      <c r="H5">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>5.89</v>
+      </c>
+      <c r="C6">
+        <v>11.66</v>
+      </c>
+      <c r="D6">
+        <v>7.74</v>
+      </c>
+      <c r="E6">
+        <v>10.44</v>
+      </c>
+      <c r="F6">
+        <v>11.79</v>
+      </c>
+      <c r="G6">
+        <v>6.67</v>
+      </c>
+      <c r="H6">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>4.25</v>
+      </c>
+      <c r="C7">
+        <v>9.59</v>
+      </c>
+      <c r="D7">
+        <v>6.13</v>
+      </c>
+      <c r="E7">
+        <v>6.39</v>
+      </c>
+      <c r="F7">
+        <v>6.83</v>
+      </c>
+      <c r="G7">
+        <v>5.08</v>
+      </c>
+      <c r="H7">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>5.44</v>
+      </c>
+      <c r="C8">
+        <v>10.29</v>
+      </c>
+      <c r="D8">
+        <v>6.96</v>
+      </c>
+      <c r="E8">
+        <v>8.83</v>
+      </c>
+      <c r="F8">
+        <v>8.029999999999999</v>
+      </c>
+      <c r="G8">
+        <v>6.22</v>
+      </c>
+      <c r="H8">
+        <v>6.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>24.75</v>
+      </c>
+      <c r="C2">
+        <v>38.35</v>
+      </c>
+      <c r="D2">
+        <v>32.03</v>
+      </c>
+      <c r="E2">
+        <v>2.11</v>
+      </c>
+      <c r="F2">
+        <v>45.86</v>
+      </c>
+      <c r="G2">
+        <v>13.1</v>
+      </c>
+      <c r="H2">
+        <v>29.69</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>13.79</v>
+      </c>
+      <c r="C3">
+        <v>18.54</v>
+      </c>
+      <c r="D3">
+        <v>28.32</v>
+      </c>
+      <c r="E3">
+        <v>14.32</v>
+      </c>
+      <c r="F3">
+        <v>16.23</v>
+      </c>
+      <c r="G3">
+        <v>9.93</v>
+      </c>
+      <c r="H3">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>11.76</v>
+      </c>
+      <c r="C4">
+        <v>16.08</v>
+      </c>
+      <c r="D4">
+        <v>24.26</v>
+      </c>
+      <c r="E4">
+        <v>9.41</v>
+      </c>
+      <c r="F4">
+        <v>15.61</v>
+      </c>
+      <c r="G4">
+        <v>7.23</v>
+      </c>
+      <c r="H4">
+        <v>14.09</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>13.08</v>
+      </c>
+      <c r="C5">
+        <v>16.19</v>
+      </c>
+      <c r="D5">
+        <v>25.05</v>
+      </c>
+      <c r="E5">
+        <v>15.15</v>
+      </c>
+      <c r="F5">
+        <v>21.4</v>
+      </c>
+      <c r="G5">
+        <v>10.6</v>
+      </c>
+      <c r="H5">
+        <v>18.56</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>15.76</v>
+      </c>
+      <c r="C6">
+        <v>23.46</v>
+      </c>
+      <c r="D6">
+        <v>24.91</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>27.77</v>
+      </c>
+      <c r="G6">
+        <v>12.64</v>
+      </c>
+      <c r="H6">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>6.76</v>
+      </c>
+      <c r="C7">
+        <v>12.5</v>
+      </c>
+      <c r="D7">
+        <v>24.21</v>
+      </c>
+      <c r="E7">
+        <v>9.44</v>
+      </c>
+      <c r="F7">
+        <v>2.83</v>
+      </c>
+      <c r="G7">
+        <v>7.34</v>
+      </c>
+      <c r="H7">
+        <v>14.58</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>13.17</v>
+      </c>
+      <c r="C8">
+        <v>18.7</v>
+      </c>
+      <c r="D8">
+        <v>26.84</v>
+      </c>
+      <c r="E8">
+        <v>13.58</v>
+      </c>
+      <c r="F8">
+        <v>18.41</v>
+      </c>
+      <c r="G8">
+        <v>9.470000000000001</v>
+      </c>
+      <c r="H8">
+        <v>18.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>

</xml_diff>

<commit_message>
3 tables from RECBR done, 7 to go...
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -19,6 +19,9 @@
     <sheet name="Figure_39" sheetId="10" r:id="rId10"/>
     <sheet name="Figure_40" sheetId="11" r:id="rId11"/>
     <sheet name="Figure_41" sheetId="12" r:id="rId12"/>
+    <sheet name="Total_Population" sheetId="13" r:id="rId13"/>
+    <sheet name="Race_Ethnicity" sheetId="14" r:id="rId14"/>
+    <sheet name="Age" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -362,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -509,6 +512,42 @@
       <c r="B12" t="inlineStr">
         <is>
           <t>Figure 41. Working Poor by Race and Ethnicity</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total_Population</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Total Population by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Race_Ethnicity</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Race/Ethnicity Distribution (%) by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Age Distribution (%) by County and SCAG Region</t>
         </is>
       </c>
     </row>
@@ -1270,6 +1309,669 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_pop</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>179943</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>10019738</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>3182954</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2409370</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>2170489</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>844838</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>18807332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1.33</v>
+      </c>
+      <c r="C2">
+        <v>14.76</v>
+      </c>
+      <c r="D2">
+        <v>21.37</v>
+      </c>
+      <c r="E2">
+        <v>6.77</v>
+      </c>
+      <c r="F2">
+        <v>7.56</v>
+      </c>
+      <c r="G2">
+        <v>7.32</v>
+      </c>
+      <c r="H2">
+        <v>13.56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>2.47</v>
+      </c>
+      <c r="C3">
+        <v>7.69</v>
+      </c>
+      <c r="D3">
+        <v>1.57</v>
+      </c>
+      <c r="E3">
+        <v>6.18</v>
+      </c>
+      <c r="F3">
+        <v>7.61</v>
+      </c>
+      <c r="G3">
+        <v>1.7</v>
+      </c>
+      <c r="H3">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>85.04000000000001</v>
+      </c>
+      <c r="C4">
+        <v>48.7</v>
+      </c>
+      <c r="D4">
+        <v>34.02</v>
+      </c>
+      <c r="E4">
+        <v>50.28</v>
+      </c>
+      <c r="F4">
+        <v>54.59</v>
+      </c>
+      <c r="G4">
+        <v>43.3</v>
+      </c>
+      <c r="H4">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.66</v>
+      </c>
+      <c r="C5">
+        <v>3.18</v>
+      </c>
+      <c r="D5">
+        <v>3.86</v>
+      </c>
+      <c r="E5">
+        <v>3.22</v>
+      </c>
+      <c r="F5">
+        <v>3.31</v>
+      </c>
+      <c r="G5">
+        <v>3.29</v>
+      </c>
+      <c r="H5">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0.15</v>
+      </c>
+      <c r="E6">
+        <v>0.35</v>
+      </c>
+      <c r="F6">
+        <v>0.31</v>
+      </c>
+      <c r="G6">
+        <v>0.22</v>
+      </c>
+      <c r="H6">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="C7">
+        <v>25.47</v>
+      </c>
+      <c r="D7">
+        <v>39.03</v>
+      </c>
+      <c r="E7">
+        <v>33.21</v>
+      </c>
+      <c r="F7">
+        <v>26.62</v>
+      </c>
+      <c r="G7">
+        <v>44.17</v>
+      </c>
+      <c r="H7">
+        <v>29.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>age_categories</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>percentages</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>21.64</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>21.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>25.16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>26.43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>22.87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>&lt;18 years</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>22.82</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>58.46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>64.66</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>63.18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>60.49</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>61.98</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>61.48</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>18 - 64 years</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>63.36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>12.84</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>14.85</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>11.59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>65+ years</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>13.82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>

</xml_diff>

<commit_message>
EOD Monday 2/12- 6 RECBR tables left to reproduce and create output
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -22,6 +22,7 @@
     <sheet name="Total_Population" sheetId="13" r:id="rId13"/>
     <sheet name="Race_Ethnicity" sheetId="14" r:id="rId14"/>
     <sheet name="Age" sheetId="15" r:id="rId15"/>
+    <sheet name="Singe_Parent_HHs" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -365,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -548,6 +549,18 @@
       <c r="B15" t="inlineStr">
         <is>
           <t>Age Distribution (%) by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Singe_Parent_HHs</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Single Parent Households (%) by Gender of Head of Household and then by County and SCAG Region</t>
         </is>
       </c>
     </row>
@@ -1972,6 +1985,246 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>single_parent_households</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>percentages</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>11.26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>female_hh</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>male_hh</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>1.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>

</xml_diff>

<commit_message>
Renamed all output tables .csv's, and completed natl origin table.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -23,6 +23,7 @@
     <sheet name="Race_Ethnicity" sheetId="14" r:id="rId14"/>
     <sheet name="Age" sheetId="15" r:id="rId15"/>
     <sheet name="Singe_Parent_HHs" sheetId="16" r:id="rId16"/>
+    <sheet name="Natl_Origin" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -366,7 +367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,6 +562,18 @@
       <c r="B16" t="inlineStr">
         <is>
           <t>Single Parent Households (%) by Gender of Head of Household and then by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Natl_Origin</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>National Origin (% Foreign born) by County and SCAG Region</t>
         </is>
       </c>
     </row>
@@ -2225,6 +2238,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>natl_origin_perc</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>29.32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>29.76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>33.51</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>29.86</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>21.55</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>20.92</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>21.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>

</xml_diff>

<commit_message>
Completed 2 more tables, 4 to go from RECBR...
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -24,6 +24,7 @@
     <sheet name="Age" sheetId="15" r:id="rId15"/>
     <sheet name="Singe_Parent_HHs" sheetId="16" r:id="rId16"/>
     <sheet name="Natl_Origin" sheetId="17" r:id="rId17"/>
+    <sheet name="LEP" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -367,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -574,6 +575,18 @@
       <c r="B17" t="inlineStr">
         <is>
           <t>National Origin (% Foreign born) by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>LEP</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Limited English Proficiency (%) by County and SCAG Region</t>
         </is>
       </c>
     </row>
@@ -2261,71 +2274,166 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SCAG</t>
+          <t>Imperial</t>
         </is>
       </c>
       <c r="B2">
-        <v>29.32</v>
+        <v>29.76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Imperial</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="B3">
-        <v>29.76</v>
+        <v>33.51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B4">
-        <v>33.51</v>
+        <v>29.86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Riverside</t>
         </is>
       </c>
       <c r="B5">
-        <v>29.86</v>
+        <v>21.55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Riverside</t>
+          <t>San Bernardino</t>
         </is>
       </c>
       <c r="B6">
-        <v>21.55</v>
+        <v>20.92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>San Bernardino</t>
+          <t>Ventura</t>
         </is>
       </c>
       <c r="B7">
-        <v>20.92</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>29.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>lep_perc</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>18.31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Ventura</t>
         </is>
       </c>
+      <c r="B7">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
       <c r="B8">
-        <v>21.2</v>
+        <v>10.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code from EOD Tues. 2/13, 3 tables left to go...
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -25,6 +25,8 @@
     <sheet name="Singe_Parent_HHs" sheetId="16" r:id="rId16"/>
     <sheet name="Natl_Origin" sheetId="17" r:id="rId17"/>
     <sheet name="LEP" sheetId="18" r:id="rId18"/>
+    <sheet name="Disablity" sheetId="19" r:id="rId19"/>
+    <sheet name="Categories_Disablity" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -368,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -587,6 +589,30 @@
       <c r="B18" t="inlineStr">
         <is>
           <t>Limited English Proficiency (%) by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Disablity</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>People with Disabilities (%) by County and SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Categories_Disablity</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Disabilites by 6 categories (%) and then by County and SCAG Region: Self-care, Hearing, Vision, Independent, Ambulatory, Cognitive</t>
         </is>
       </c>
     </row>
@@ -2441,6 +2467,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dis_perc</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>14.44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>10.42</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>8.880000000000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>11.18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>10.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>
@@ -2685,6 +2806,666 @@
       </c>
       <c r="H8">
         <v>6.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>disability_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Self-care difficulty</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Hearing difficulty</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>2.03</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>2.03</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Vision difficulty</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Independent living</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>4.48</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>4.39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Ambulatory difficulty</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>4.31</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>4.9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>4.27</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Cognitive difficulty</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>4.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Brief update, 2 tables left to go.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -27,6 +27,7 @@
     <sheet name="LEP" sheetId="18" r:id="rId18"/>
     <sheet name="Disablity" sheetId="19" r:id="rId19"/>
     <sheet name="Categories_Disablity" sheetId="20" r:id="rId20"/>
+    <sheet name="Education" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -370,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -613,6 +614,18 @@
       <c r="B20" t="inlineStr">
         <is>
           <t>Disabilites by 6 categories (%) and then by County and SCAG Region: Self-care, Hearing, Vision, Independent, Ambulatory, Cognitive</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Educational Attainment (%) by Race/ethincity and whole SCAG Region</t>
         </is>
       </c>
     </row>
@@ -3473,6 +3486,666 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>edu</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>10.97</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>9.33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>34.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>4.67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Less than HS Diploma</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>18.45</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>27.57</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>18.18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>HS Diploma</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>13.47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>28.85</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>18.67</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>23.55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>27.39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>22.47</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Some College</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>19.99</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>9.91</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AA Degree</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>7.59</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>35.78</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>18.07</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>28.89</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>13.43</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>27.71</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BA degree</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>20.86</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>17.78</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>10.24</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>4.06</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>16.91</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>MA degree or higher</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>11.63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>

</xml_diff>

<commit_message>
Fixed figure 20 to match SAS output- doesn't match figure from Equity_Report_Figures_20231102.xlsx- need to note.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -3497,7 +3497,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>edu</t>
+          <t>education_level</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -6059,19 +6059,19 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.91</v>
+        <v>2.26</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3">
@@ -6081,25 +6081,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="C3">
-        <v>0.32</v>
+        <v>0.53</v>
       </c>
       <c r="D3">
-        <v>0.25</v>
+        <v>0.29</v>
       </c>
       <c r="E3">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
       <c r="F3">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="G3">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="H3">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="4">
@@ -6109,25 +6109,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="C4">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="E4">
-        <v>0.26</v>
+        <v>0.41</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="H4">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="5">
@@ -6137,25 +6137,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.04</v>
+        <v>0.12</v>
       </c>
       <c r="C5">
         <v>0.14</v>
       </c>
       <c r="D5">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E5">
-        <v>0.26</v>
+        <v>0.3</v>
       </c>
       <c r="F5">
-        <v>1.63</v>
+        <v>1.79</v>
       </c>
       <c r="G5">
+        <v>0.18</v>
+      </c>
+      <c r="H5">
         <v>0.19</v>
-      </c>
-      <c r="H5">
-        <v>0.17</v>
       </c>
     </row>
     <row r="6">
@@ -6165,25 +6165,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.39</v>
+        <v>0.31</v>
       </c>
       <c r="C6">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="D6">
+        <v>0.18</v>
+      </c>
+      <c r="E6">
         <v>0.14</v>
       </c>
-      <c r="E6">
-        <v>0.12</v>
-      </c>
       <c r="F6">
-        <v>0.21</v>
+        <v>0.53</v>
       </c>
       <c r="G6">
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="H6">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="7">
@@ -6199,19 +6199,19 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.11</v>
+        <v>0.18</v>
       </c>
       <c r="E7">
-        <v>0.09</v>
+        <v>0.33</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.15</v>
+        <v>0.26</v>
       </c>
       <c r="H7">
-        <v>0.13</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="8">
@@ -6221,25 +6221,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="C8">
-        <v>0.28</v>
+        <v>0.42</v>
       </c>
       <c r="D8">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="E8">
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
       <c r="F8">
-        <v>0.41</v>
+        <v>0.54</v>
       </c>
       <c r="G8">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="H8">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All tables replicated, need to change all to long form.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -28,6 +28,8 @@
     <sheet name="Disablity" sheetId="19" r:id="rId19"/>
     <sheet name="Categories_Disablity" sheetId="20" r:id="rId20"/>
     <sheet name="Education" sheetId="21" r:id="rId21"/>
+    <sheet name="Median_HH_Income" sheetId="22" r:id="rId22"/>
+    <sheet name="Poverty_HH" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -371,7 +373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -626,6 +628,30 @@
       <c r="B21" t="inlineStr">
         <is>
           <t>Educational Attainment (%) by Race/ethincity and whole SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Median_HH_Income</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Median Household Income by Race/ethincity and whole SCAG Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Poverty_HH</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Household Poverty (%) by Race/ethincity and whole SCAG Region</t>
         </is>
       </c>
     </row>
@@ -4146,6 +4172,196 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>med_hh_income</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>93517.74000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>57918.45</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>66943.16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>86696.87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>65439.84</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>96171.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG region</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>79645.22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>25.42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>37.09</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>38.39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>35.52</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>28.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>

</xml_diff>

<commit_message>
All tables in scag_tabbed.xlsx in long form and adjusted column widths. Next, need to clean code. Last, commit with full code included.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -1,42 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" firstSheet="0" windowHeight="13125" windowWidth="13125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TOC" sheetId="1" r:id="rId1"/>
-    <sheet name="Figure_5" sheetId="2" r:id="rId2"/>
-    <sheet name="Figure_6" sheetId="3" r:id="rId3"/>
-    <sheet name="Figure_7" sheetId="4" r:id="rId4"/>
-    <sheet name="Figure_19" sheetId="5" r:id="rId5"/>
-    <sheet name="Figure_20" sheetId="6" r:id="rId6"/>
-    <sheet name="Figure_21" sheetId="7" r:id="rId7"/>
-    <sheet name="Figure_22" sheetId="8" r:id="rId8"/>
-    <sheet name="Figure_28" sheetId="9" r:id="rId9"/>
-    <sheet name="Figure_39" sheetId="10" r:id="rId10"/>
-    <sheet name="Figure_40" sheetId="11" r:id="rId11"/>
-    <sheet name="Figure_41" sheetId="12" r:id="rId12"/>
-    <sheet name="Total_Population" sheetId="13" r:id="rId13"/>
-    <sheet name="Race_Ethnicity" sheetId="14" r:id="rId14"/>
-    <sheet name="Age" sheetId="15" r:id="rId15"/>
-    <sheet name="Singe_Parent_HHs" sheetId="16" r:id="rId16"/>
-    <sheet name="Natl_Origin" sheetId="17" r:id="rId17"/>
-    <sheet name="LEP" sheetId="18" r:id="rId18"/>
-    <sheet name="Disablity" sheetId="19" r:id="rId19"/>
-    <sheet name="Categories_Disablity" sheetId="20" r:id="rId20"/>
-    <sheet name="Education" sheetId="21" r:id="rId21"/>
-    <sheet name="Median_HH_Income" sheetId="22" r:id="rId22"/>
-    <sheet name="Poverty_HH" sheetId="23" r:id="rId23"/>
+    <sheet name="TOC" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Figure_5" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Figure_6" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Figure_7" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Figure_19" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Figure_20" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Figure_21" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Figure_22" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Figure_28" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Figure_39" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Figure_40" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Figure_41" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Total_Population" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Race_Ethnicity" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Age" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Singe_Parent_HHs" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Natl_Origin" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="LEP" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Disablity" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Categories_Disablity" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Education" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Median_HH_Income" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Poverty_HH" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -46,12 +44,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,9 +70,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -84,7 +81,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -99,44 +95,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -163,14 +159,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -197,6 +211,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -208,184 +240,164 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="20.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="130.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>sheet_name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>figure_name</t>
         </is>
@@ -656,30 +668,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="11.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>med_hr_wage</t>
         </is>
@@ -1421,30 +1440,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="15.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>unemployed_perc</t>
         </is>
@@ -1507,7 +1533,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>9.800000000000001</v>
+        <v>9.8</v>
       </c>
     </row>
     <row r="6">
@@ -1717,7 +1743,7 @@
         </is>
       </c>
       <c r="C19">
-        <v>8.289999999999999</v>
+        <v>8.29</v>
       </c>
     </row>
     <row r="20">
@@ -2152,7 +2178,7 @@
         </is>
       </c>
       <c r="C48">
-        <v>8.029999999999999</v>
+        <v>8.03</v>
       </c>
     </row>
     <row r="49">
@@ -2186,57 +2212,39 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="23.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Asian/Pacific Islander</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Black</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Hispanic/Latino</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Multiracial/Other</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Native American</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>White</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>working_poor_percentage</t>
         </is>
       </c>
     </row>
@@ -2246,218 +2254,763 @@
           <t>Imperial</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C2">
         <v>24.75</v>
-      </c>
-      <c r="C2">
-        <v>38.35</v>
-      </c>
-      <c r="D2">
-        <v>32.03</v>
-      </c>
-      <c r="E2">
-        <v>2.11</v>
-      </c>
-      <c r="F2">
-        <v>45.86</v>
-      </c>
-      <c r="G2">
-        <v>13.1</v>
-      </c>
-      <c r="H2">
-        <v>29.69</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>13.79</v>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
       </c>
       <c r="C3">
-        <v>18.54</v>
-      </c>
-      <c r="D3">
-        <v>28.32</v>
-      </c>
-      <c r="E3">
-        <v>14.32</v>
-      </c>
-      <c r="F3">
-        <v>16.23</v>
-      </c>
-      <c r="G3">
-        <v>9.93</v>
-      </c>
-      <c r="H3">
-        <v>19.9</v>
+        <v>38.35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>11.76</v>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
       </c>
       <c r="C4">
-        <v>16.08</v>
-      </c>
-      <c r="D4">
-        <v>24.26</v>
-      </c>
-      <c r="E4">
-        <v>9.41</v>
-      </c>
-      <c r="F4">
-        <v>15.61</v>
-      </c>
-      <c r="G4">
-        <v>7.23</v>
-      </c>
-      <c r="H4">
-        <v>14.09</v>
+        <v>32.03</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Riverside</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>13.08</v>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
       </c>
       <c r="C5">
-        <v>16.19</v>
-      </c>
-      <c r="D5">
-        <v>25.05</v>
-      </c>
-      <c r="E5">
-        <v>15.15</v>
-      </c>
-      <c r="F5">
-        <v>21.4</v>
-      </c>
-      <c r="G5">
-        <v>10.6</v>
-      </c>
-      <c r="H5">
-        <v>18.56</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>San Bernardino</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>15.76</v>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
       </c>
       <c r="C6">
-        <v>23.46</v>
-      </c>
-      <c r="D6">
-        <v>24.91</v>
-      </c>
-      <c r="E6">
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <v>27.77</v>
-      </c>
-      <c r="G6">
-        <v>12.64</v>
-      </c>
-      <c r="H6">
-        <v>20.49</v>
+        <v>45.86</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ventura</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>6.76</v>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
       </c>
       <c r="C7">
-        <v>12.5</v>
-      </c>
-      <c r="D7">
-        <v>24.21</v>
-      </c>
-      <c r="E7">
-        <v>9.44</v>
-      </c>
-      <c r="F7">
-        <v>2.83</v>
-      </c>
-      <c r="G7">
-        <v>7.34</v>
-      </c>
-      <c r="H7">
-        <v>14.58</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>29.69</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>13.79</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>18.54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>28.32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>14.32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>16.23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>9.93</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>11.76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>16.08</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>24.26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>9.41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>14.09</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>13.08</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>16.19</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>25.05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>18.56</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>23.46</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>24.91</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>27.77</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>12.64</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>24.21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>14.58</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>SCAG</t>
         </is>
       </c>
-      <c r="B8">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C44">
         <v>13.17</v>
       </c>
-      <c r="C8">
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C45">
         <v>18.7</v>
       </c>
-      <c r="D8">
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C46">
         <v>26.84</v>
       </c>
-      <c r="E8">
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C47">
         <v>13.58</v>
       </c>
-      <c r="F8">
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C48">
         <v>18.41</v>
       </c>
-      <c r="G8">
-        <v>9.470000000000001</v>
-      </c>
-      <c r="H8">
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>9.47</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SCAG Region</t>
+        </is>
+      </c>
+      <c r="C50">
         <v>18.6</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="16.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>total_pop</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>total_population</t>
         </is>
       </c>
     </row>
@@ -2532,255 +3085,705 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="15.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Imperial</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Riverside</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>San Bernardino</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Ventura</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>SCAG</t>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>race_percentage</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Asian/Pacific Islander</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>1.33</v>
-      </c>
-      <c r="C2">
-        <v>14.76</v>
-      </c>
-      <c r="D2">
-        <v>21.37</v>
-      </c>
-      <c r="E2">
-        <v>6.77</v>
-      </c>
-      <c r="F2">
-        <v>7.56</v>
-      </c>
-      <c r="G2">
-        <v>7.32</v>
-      </c>
-      <c r="H2">
-        <v>13.56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Black</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2.47</v>
-      </c>
-      <c r="C3">
-        <v>7.69</v>
-      </c>
-      <c r="D3">
-        <v>1.57</v>
-      </c>
-      <c r="E3">
-        <v>6.18</v>
-      </c>
-      <c r="F3">
-        <v>7.61</v>
-      </c>
-      <c r="G3">
-        <v>1.7</v>
-      </c>
-      <c r="H3">
-        <v>6.13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Hispanic/Latino</t>
         </is>
       </c>
-      <c r="B4">
-        <v>85.04000000000001</v>
-      </c>
       <c r="C4">
-        <v>48.7</v>
-      </c>
-      <c r="D4">
-        <v>34.02</v>
-      </c>
-      <c r="E4">
-        <v>50.28</v>
-      </c>
-      <c r="F4">
-        <v>54.59</v>
-      </c>
-      <c r="G4">
-        <v>43.3</v>
-      </c>
-      <c r="H4">
-        <v>47.2</v>
+        <v>85.04</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Multiracial/Other</t>
         </is>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.66</v>
-      </c>
-      <c r="C5">
-        <v>3.18</v>
-      </c>
-      <c r="D5">
-        <v>3.86</v>
-      </c>
-      <c r="E5">
-        <v>3.22</v>
-      </c>
-      <c r="F5">
-        <v>3.31</v>
-      </c>
-      <c r="G5">
-        <v>3.29</v>
-      </c>
-      <c r="H5">
-        <v>3.29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Native American</t>
         </is>
       </c>
-      <c r="B6">
-        <v>0.6899999999999999</v>
-      </c>
       <c r="C6">
-        <v>0.2</v>
-      </c>
-      <c r="D6">
-        <v>0.15</v>
-      </c>
-      <c r="E6">
-        <v>0.35</v>
-      </c>
-      <c r="F6">
-        <v>0.31</v>
-      </c>
-      <c r="G6">
-        <v>0.22</v>
-      </c>
-      <c r="H6">
-        <v>0.23</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Imperial</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>White</t>
         </is>
       </c>
-      <c r="B7">
-        <v>9.800000000000001</v>
-      </c>
       <c r="C7">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>14.76</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>7.69</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>48.7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C13">
         <v>25.47</v>
       </c>
-      <c r="D7">
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>21.37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>34.02</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C19">
         <v>39.03</v>
       </c>
-      <c r="E7">
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>6.77</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>50.28</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C25">
         <v>33.21</v>
       </c>
-      <c r="F7">
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>7.61</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>54.59</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>San Bernardino</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C31">
         <v>26.62</v>
       </c>
-      <c r="G7">
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Ventura</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C37">
         <v>44.17</v>
       </c>
-      <c r="H7">
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Asian/Pacific Islander</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>13.56</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Hispanic/Latino</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Multiracial/Other</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Native American</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C43">
         <v>29.58</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="10.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>age_categories</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>percentages</t>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>percentage</t>
         </is>
       </c>
     </row>
@@ -3100,32 +4103,39 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="24.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="27.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>single_parent_households</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>gender_head_of_household</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>percentages</t>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>single_parent_hh_percentage</t>
         </is>
       </c>
     </row>
@@ -3340,27 +4350,33 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="23.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>natl_origin_perc</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>foreign_born_percentage</t>
         </is>
       </c>
     </row>
@@ -3435,27 +4451,33 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="38.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>lep_perc</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>limited_english_proficiency_percentage</t>
         </is>
       </c>
     </row>
@@ -3530,27 +4552,33 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="23.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>dis_perc</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>disabilities_percentage</t>
         </is>
       </c>
     </row>
@@ -3581,7 +4609,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>8.880000000000001</v>
+        <v>8.88</v>
       </c>
     </row>
     <row r="5">
@@ -3625,30 +4653,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="27.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>walk_bike_public_percentage</t>
         </is>
@@ -3801,7 +4836,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>9.960000000000001</v>
+        <v>9.96</v>
       </c>
     </row>
     <row r="12">
@@ -3816,7 +4851,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>9.789999999999999</v>
+        <v>9.79</v>
       </c>
     </row>
     <row r="13">
@@ -3831,7 +4866,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>9.550000000000001</v>
+        <v>9.55</v>
       </c>
     </row>
     <row r="14">
@@ -4356,7 +5391,7 @@
         </is>
       </c>
       <c r="C48">
-        <v>8.800000000000001</v>
+        <v>8.8</v>
       </c>
     </row>
     <row r="49">
@@ -4390,30 +5425,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="21.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="10.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>disability_type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>percentage</t>
         </is>
@@ -5050,30 +6092,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="20.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="10.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>education_level</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>percentage</t>
         </is>
@@ -5177,7 +6226,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SCAG region</t>
+          <t>SCAG Region</t>
         </is>
       </c>
       <c r="C8">
@@ -5282,7 +6331,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SCAG region</t>
+          <t>SCAG Region</t>
         </is>
       </c>
       <c r="C15">
@@ -5387,7 +6436,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SCAG region</t>
+          <t>SCAG Region</t>
         </is>
       </c>
       <c r="C22">
@@ -5492,7 +6541,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SCAG region</t>
+          <t>SCAG Region</t>
         </is>
       </c>
       <c r="C29">
@@ -5597,7 +6646,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SCAG region</t>
+          <t>SCAG Region</t>
         </is>
       </c>
       <c r="C36">
@@ -5702,7 +6751,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SCAG region</t>
+          <t>SCAG Region</t>
         </is>
       </c>
       <c r="C43">
@@ -5710,27 +6759,33 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="23.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>med_hh_income</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>median_household_income</t>
         </is>
       </c>
     </row>
@@ -5741,7 +6796,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>93517.74000000001</v>
+        <v>93517.74</v>
       </c>
     </row>
     <row r="3">
@@ -5805,27 +6860,33 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="28.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>percentage</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>household_poverty_percentage</t>
         </is>
       </c>
     </row>
@@ -5900,30 +6961,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="21.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>no_vehicle_percentage</t>
         </is>
@@ -6046,7 +7114,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>8.220000000000001</v>
+        <v>8.22</v>
       </c>
     </row>
     <row r="10">
@@ -6091,7 +7159,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>8.869999999999999</v>
+        <v>8.87</v>
       </c>
     </row>
     <row r="13">
@@ -6136,7 +7204,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>8.619999999999999</v>
+        <v>8.62</v>
       </c>
     </row>
     <row r="16">
@@ -6650,35 +7718,43 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="19.711"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" hidden="false" width="29.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>transportation_type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>mean_transit_times_in_minutes</t>
         </is>
@@ -8261,7 +9337,7 @@
         </is>
       </c>
       <c r="D80">
-        <v>64.06999999999999</v>
+        <v>64.07</v>
       </c>
     </row>
     <row r="81">
@@ -8661,7 +9737,7 @@
         </is>
       </c>
       <c r="D100">
-        <v>67.23999999999999</v>
+        <v>67.24</v>
       </c>
     </row>
     <row r="101">
@@ -8821,7 +9897,7 @@
         </is>
       </c>
       <c r="D108">
-        <v>64.95999999999999</v>
+        <v>64.96</v>
       </c>
     </row>
     <row r="109">
@@ -8901,7 +9977,7 @@
         </is>
       </c>
       <c r="D112">
-        <v>85.56999999999999</v>
+        <v>85.57</v>
       </c>
     </row>
     <row r="113">
@@ -10125,35 +11201,42 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" hidden="false" width="17.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>household_type</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>burden_percentage</t>
         </is>
@@ -11156,7 +12239,7 @@
         </is>
       </c>
       <c r="D51">
-        <v>9.130000000000001</v>
+        <v>9.13</v>
       </c>
     </row>
     <row r="52">
@@ -11256,7 +12339,7 @@
         </is>
       </c>
       <c r="D56">
-        <v>8.470000000000001</v>
+        <v>8.47</v>
       </c>
     </row>
     <row r="57">
@@ -11556,7 +12639,7 @@
         </is>
       </c>
       <c r="D71">
-        <v>8.640000000000001</v>
+        <v>8.64</v>
       </c>
     </row>
     <row r="72">
@@ -11916,7 +12999,7 @@
         </is>
       </c>
       <c r="D89">
-        <v>8.470000000000001</v>
+        <v>8.47</v>
       </c>
     </row>
     <row r="90">
@@ -12120,30 +13203,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="30.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>no_kitchen_plumbing_percentage</t>
         </is>
@@ -12885,30 +13975,36 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="3" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>overcrowded_percentage</t>
         </is>
@@ -12941,7 +14037,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>9.720000000000001</v>
+        <v>9.72</v>
       </c>
     </row>
     <row r="4">
@@ -13635,30 +14731,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="24.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>homeownership_percentage</t>
         </is>
@@ -13721,7 +14824,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>75.68000000000001</v>
+        <v>75.68</v>
       </c>
     </row>
     <row r="6">
@@ -13736,7 +14839,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>65.54000000000001</v>
+        <v>65.54</v>
       </c>
     </row>
     <row r="7">
@@ -13961,7 +15064,7 @@
         </is>
       </c>
       <c r="C21">
-        <v>64.56999999999999</v>
+        <v>64.57</v>
       </c>
     </row>
     <row r="22">
@@ -14096,7 +15199,7 @@
         </is>
       </c>
       <c r="C30">
-        <v>69.15000000000001</v>
+        <v>69.15</v>
       </c>
     </row>
     <row r="31">
@@ -14201,7 +15304,7 @@
         </is>
       </c>
       <c r="C37">
-        <v>76.79000000000001</v>
+        <v>76.79</v>
       </c>
     </row>
     <row r="38">
@@ -14400,30 +15503,37 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="22.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="30.711"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>county</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>no_health_insurance_percentage</t>
         </is>
@@ -14441,7 +15551,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>8.220000000000001</v>
+        <v>8.22</v>
       </c>
     </row>
     <row r="3">
@@ -14456,7 +15566,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>8.220000000000001</v>
+        <v>8.22</v>
       </c>
     </row>
     <row r="4">
@@ -14486,7 +15596,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>9.449999999999999</v>
+        <v>9.45</v>
       </c>
     </row>
     <row r="6">
@@ -14846,7 +15956,7 @@
         </is>
       </c>
       <c r="C29">
-        <v>8.460000000000001</v>
+        <v>8.46</v>
       </c>
     </row>
     <row r="30">
@@ -14876,7 +15986,7 @@
         </is>
       </c>
       <c r="C31">
-        <v>9.550000000000001</v>
+        <v>9.55</v>
       </c>
     </row>
     <row r="32">
@@ -15165,6 +16275,8 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last update before consolidating/streamlining code- from this point on code will on be what is necesary to run and produce output.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -39,14 +39,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -95,39 +95,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -179,7 +179,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -290,13 +290,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -305,6 +298,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -369,11 +369,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -402,6 +422,9 @@
           <t>figure_name</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -676,7 +699,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -703,6 +726,8 @@
           <t>med_hr_wage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1448,7 +1473,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -1475,6 +1500,8 @@
           <t>unemployed_perc</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2220,7 +2247,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -2247,6 +2274,8 @@
           <t>working_poor_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2992,7 +3021,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -3013,6 +3042,9 @@
           <t>total_population</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3093,7 +3125,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -3120,6 +3152,8 @@
           <t>race_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3760,7 +3794,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -3786,6 +3820,8 @@
           <t>percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4111,7 +4147,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -4138,6 +4174,8 @@
           <t>single_parent_hh_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4358,7 +4396,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -4379,6 +4417,9 @@
           <t>foreign_born_percentage</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4459,7 +4500,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -4480,6 +4521,9 @@
           <t>limited_english_proficiency_percentage</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4560,7 +4604,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -4581,6 +4625,9 @@
           <t>disabilities_percentage</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4661,7 +4708,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -4688,6 +4735,8 @@
           <t>walk_bike_public_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5433,7 +5482,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -5460,6 +5509,8 @@
           <t>percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6100,7 +6151,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -6127,6 +6178,8 @@
           <t>percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6767,7 +6820,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -6788,6 +6841,9 @@
           <t>median_household_income</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6868,7 +6924,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -6889,6 +6945,9 @@
           <t>household_poverty_percentage</t>
         </is>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6969,7 +7028,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -6996,6 +7055,8 @@
           <t>no_vehicle_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7726,7 +7787,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -7759,6 +7820,7 @@
           <t>mean_transit_times_in_minutes</t>
         </is>
       </c>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -11209,7 +11271,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -11241,6 +11303,7 @@
           <t>burden_percentage</t>
         </is>
       </c>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -13211,7 +13274,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -13238,6 +13301,8 @@
           <t>no_kitchen_plumbing_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -13983,7 +14048,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -14009,6 +14074,8 @@
           <t>overcrowded_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -14739,7 +14806,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -14766,6 +14833,8 @@
           <t>homeownership_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -15511,7 +15580,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -15538,6 +15607,8 @@
           <t>no_health_insurance_percentage</t>
         </is>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
In order to use both 2017-21 or 2018-22 datasets, need to change cleaning to accomdate differences- mostly adjusted income different by year, last commit before changing.
</commit_message>
<xml_diff>
--- a/output/scag_tabbed.xlsx
+++ b/output/scag_tabbed.xlsx
@@ -419,7 +419,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>figure_name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="C1" s="2"/>
@@ -13623,7 +13623,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -14246,11 +14246,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C41">
-        <v>4.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -14261,26 +14261,26 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C42">
-        <v>4.1</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SCAG</t>
+          <t>Ventura</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C43">
-        <v>6.97</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="44">
@@ -14291,11 +14291,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C44">
-        <v>13.7</v>
+        <v>6.97</v>
       </c>
     </row>
     <row r="45">
@@ -14306,11 +14306,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C45">
-        <v>6.31</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="46">
@@ -14321,11 +14321,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C46">
-        <v>7.13</v>
+        <v>6.31</v>
       </c>
     </row>
     <row r="47">
@@ -14336,11 +14336,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C47">
-        <v>11.05</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="48">
@@ -14351,11 +14351,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C48">
-        <v>5.68</v>
+        <v>11.05</v>
       </c>
     </row>
     <row r="49">
@@ -14366,10 +14366,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>All Races</t>
         </is>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>6.71</v>
       </c>
     </row>
@@ -21124,7 +21139,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -21206,11 +21221,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C5">
-        <v>3.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -21221,11 +21236,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C6">
-        <v>0.57</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="7">
@@ -21236,26 +21251,26 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C7">
-        <v>4.58</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Imperial</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C8">
-        <v>5.37</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="9">
@@ -21266,11 +21281,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C9">
-        <v>2.69</v>
+        <v>5.37</v>
       </c>
     </row>
     <row r="10">
@@ -21281,11 +21296,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C10">
-        <v>11.13</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="11">
@@ -21296,11 +21311,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C11">
-        <v>2.95</v>
+        <v>11.13</v>
       </c>
     </row>
     <row r="12">
@@ -21311,11 +21326,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C12">
-        <v>1.56</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="13">
@@ -21326,11 +21341,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C13">
-        <v>1.58</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="14">
@@ -21341,26 +21356,26 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C14">
-        <v>5.95</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C15">
-        <v>3.65</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="16">
@@ -21371,11 +21386,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C16">
-        <v>2.46</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="17">
@@ -21386,11 +21401,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C17">
-        <v>11.31</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="18">
@@ -21401,11 +21416,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>11.31</v>
       </c>
     </row>
     <row r="19">
@@ -21416,11 +21431,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C19">
-        <v>2.17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -21431,11 +21446,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C20">
-        <v>1.2</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="21">
@@ -21446,26 +21461,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C21">
-        <v>4.25</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Riverside</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C22">
-        <v>2.79</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="23">
@@ -21476,11 +21491,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C23">
-        <v>2.18</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="24">
@@ -21491,11 +21506,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C24">
-        <v>5.58</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="25">
@@ -21506,11 +21521,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C25">
-        <v>2.74</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="26">
@@ -21521,11 +21536,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C26">
-        <v>1.14</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="27">
@@ -21536,11 +21551,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C27">
-        <v>0.77</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="28">
@@ -21551,26 +21566,26 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C28">
-        <v>2.95</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>San Bernardino</t>
+          <t>Riverside</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C29">
-        <v>3.06</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="30">
@@ -21581,11 +21596,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C30">
-        <v>2.26</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="31">
@@ -21596,11 +21611,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C31">
-        <v>5.77</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="32">
@@ -21611,11 +21626,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C32">
-        <v>2.42</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="33">
@@ -21626,11 +21641,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C33">
-        <v>2.54</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="34">
@@ -21641,11 +21656,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C34">
-        <v>1.13</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="35">
@@ -21656,26 +21671,26 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C35">
-        <v>3.52</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ventura</t>
+          <t>San Bernardino</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C36">
-        <v>2.98</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="37">
@@ -21686,11 +21701,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C37">
-        <v>2.17</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="38">
@@ -21701,11 +21716,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C38">
-        <v>7.51</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="39">
@@ -21716,11 +21731,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C39">
-        <v>1.05</v>
+        <v>7.51</v>
       </c>
     </row>
     <row r="40">
@@ -21731,11 +21746,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C40">
-        <v>0.49</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="41">
@@ -21746,11 +21761,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C41">
-        <v>0.55</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="42">
@@ -21761,26 +21776,26 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>All Races</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C42">
-        <v>2.96</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SCAG</t>
+          <t>Ventura</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Asian/Pacific Islander</t>
+          <t>All Races</t>
         </is>
       </c>
       <c r="C43">
-        <v>4.59</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="44">
@@ -21791,11 +21806,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Asian/Pacific Islander</t>
         </is>
       </c>
       <c r="C44">
-        <v>2.58</v>
+        <v>4.59</v>
       </c>
     </row>
     <row r="45">
@@ -21806,11 +21821,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Hispanic/Latino</t>
+          <t>Black</t>
         </is>
       </c>
       <c r="C45">
-        <v>9.5</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="46">
@@ -21821,11 +21836,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Multiracial/Other</t>
+          <t>Hispanic/Latino</t>
         </is>
       </c>
       <c r="C46">
-        <v>2.62</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="47">
@@ -21836,11 +21851,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Native American</t>
+          <t>Multiracial/Other</t>
         </is>
       </c>
       <c r="C47">
-        <v>1.68</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="48">
@@ -21851,11 +21866,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Native American</t>
         </is>
       </c>
       <c r="C48">
-        <v>1.27</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="49">
@@ -21866,10 +21881,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SCAG</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>All Races</t>
         </is>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>4.89</v>
       </c>
     </row>

</xml_diff>